<commit_message>
Modify the code - log squeeze
</commit_message>
<xml_diff>
--- a/output/vaginal_probability_sample_estimation.xlsx
+++ b/output/vaginal_probability_sample_estimation.xlsx
@@ -515,31 +515,31 @@
         <v>44.9</v>
       </c>
       <c r="C2" t="n">
-        <v>40.3</v>
+        <v>40.7</v>
       </c>
       <c r="D2" t="n">
-        <v>40.3</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>42.5</v>
+        <v>25.7</v>
       </c>
       <c r="F2" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>53.2</v>
+        <v>63.5</v>
       </c>
       <c r="H2" t="n">
-        <v>25.6</v>
+        <v>23.7</v>
       </c>
       <c r="I2" t="n">
-        <v>47</v>
+        <v>53.5</v>
       </c>
       <c r="J2" t="n">
-        <v>93.8</v>
+        <v>59.9</v>
       </c>
       <c r="K2" t="n">
-        <v>55.2</v>
+        <v>48.2</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -565,31 +565,31 @@
         <v>44.9</v>
       </c>
       <c r="C3" t="n">
-        <v>47.3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>95</v>
+        <v>47.4</v>
       </c>
       <c r="E3" t="n">
-        <v>41.2</v>
+        <v>51.4</v>
       </c>
       <c r="F3" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>95</v>
+        <v>30.5</v>
       </c>
       <c r="H3" t="n">
-        <v>21.6</v>
+        <v>10</v>
       </c>
       <c r="I3" t="n">
-        <v>91.59999999999999</v>
+        <v>24.7</v>
       </c>
       <c r="J3" t="n">
-        <v>56.1</v>
+        <v>55.9</v>
       </c>
       <c r="K3" t="n">
-        <v>45.3</v>
+        <v>10</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -615,31 +615,31 @@
         <v>44.9</v>
       </c>
       <c r="C4" t="n">
-        <v>46</v>
+        <v>49.8</v>
       </c>
       <c r="D4" t="n">
-        <v>31.2</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>22.8</v>
+        <v>17</v>
       </c>
       <c r="F4" t="n">
-        <v>68.3</v>
+        <v>57.1</v>
       </c>
       <c r="G4" t="n">
-        <v>50.1</v>
+        <v>46.9</v>
       </c>
       <c r="H4" t="n">
-        <v>30</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>12</v>
+        <v>37.3</v>
       </c>
       <c r="J4" t="n">
-        <v>45.3</v>
+        <v>48.8</v>
       </c>
       <c r="K4" t="n">
-        <v>24.7</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -665,31 +665,31 @@
         <v>44.9</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>41.1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>48.2</v>
+        <v>42</v>
       </c>
       <c r="G5" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H5" t="n">
-        <v>52.5</v>
+        <v>32.1</v>
       </c>
       <c r="I5" t="n">
-        <v>44.8</v>
+        <v>10</v>
       </c>
       <c r="J5" t="n">
-        <v>33.8</v>
+        <v>14.3</v>
       </c>
       <c r="K5" t="n">
-        <v>51.1</v>
+        <v>25.4</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -715,31 +715,31 @@
         <v>44.9</v>
       </c>
       <c r="C6" t="n">
-        <v>38.4</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>31.1</v>
+        <v>31</v>
       </c>
       <c r="E6" t="n">
-        <v>41.1</v>
+        <v>20.8</v>
       </c>
       <c r="F6" t="n">
-        <v>68.59999999999999</v>
+        <v>54.5</v>
       </c>
       <c r="G6" t="n">
-        <v>69.09999999999999</v>
+        <v>52.6</v>
       </c>
       <c r="H6" t="n">
-        <v>21.6</v>
+        <v>18</v>
       </c>
       <c r="I6" t="n">
-        <v>11.3</v>
+        <v>10</v>
       </c>
       <c r="J6" t="n">
-        <v>33.3</v>
+        <v>19.5</v>
       </c>
       <c r="K6" t="n">
-        <v>23.7</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -765,31 +765,31 @@
         <v>44.9</v>
       </c>
       <c r="C7" t="n">
-        <v>24.4</v>
+        <v>13.1</v>
       </c>
       <c r="D7" t="n">
-        <v>31.1</v>
+        <v>31.5</v>
       </c>
       <c r="E7" t="n">
-        <v>42</v>
+        <v>25.3</v>
       </c>
       <c r="F7" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G7" t="n">
-        <v>44.2</v>
+        <v>44.7</v>
       </c>
       <c r="H7" t="n">
-        <v>22.3</v>
+        <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>45.6</v>
+        <v>19.3</v>
       </c>
       <c r="J7" t="n">
-        <v>70.59999999999999</v>
+        <v>48.7</v>
       </c>
       <c r="K7" t="n">
-        <v>66.3</v>
+        <v>25.1</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -818,28 +818,28 @@
         <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>33.5</v>
+        <v>40.8</v>
       </c>
       <c r="E8" t="n">
-        <v>94.5</v>
+        <v>95</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>41.7</v>
       </c>
       <c r="G8" t="n">
-        <v>45.6</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>78.7</v>
+        <v>70</v>
       </c>
       <c r="I8" t="n">
-        <v>58.4</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>33.2</v>
+        <v>14.2</v>
       </c>
       <c r="K8" t="n">
-        <v>95</v>
+        <v>70.8</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -865,31 +865,31 @@
         <v>44.9</v>
       </c>
       <c r="C9" t="n">
-        <v>27.1</v>
+        <v>16.7</v>
       </c>
       <c r="D9" t="n">
-        <v>31.4</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>90.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="F9" t="n">
-        <v>57.2</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>46.1</v>
+        <v>90.8</v>
       </c>
       <c r="H9" t="n">
-        <v>40.5</v>
+        <v>58.9</v>
       </c>
       <c r="I9" t="n">
-        <v>60.7</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>33</v>
+        <v>13.9</v>
       </c>
       <c r="K9" t="n">
-        <v>45.4</v>
+        <v>19.5</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -915,31 +915,31 @@
         <v>44.9</v>
       </c>
       <c r="C10" t="n">
-        <v>58.6</v>
+        <v>70.7</v>
       </c>
       <c r="D10" t="n">
-        <v>95</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>76.7</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>14.4</v>
+        <v>89.8</v>
       </c>
       <c r="G10" t="n">
-        <v>90.5</v>
+        <v>94.5</v>
       </c>
       <c r="H10" t="n">
-        <v>67.09999999999999</v>
+        <v>88.3</v>
       </c>
       <c r="I10" t="n">
-        <v>91.59999999999999</v>
+        <v>85.7</v>
       </c>
       <c r="J10" t="n">
-        <v>33.3</v>
+        <v>27</v>
       </c>
       <c r="K10" t="n">
-        <v>46.5</v>
+        <v>49.1</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -965,31 +965,31 @@
         <v>44.9</v>
       </c>
       <c r="C11" t="n">
-        <v>21.6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>31.1</v>
+        <v>31.9</v>
       </c>
       <c r="E11" t="n">
-        <v>42.4</v>
+        <v>53.5</v>
       </c>
       <c r="F11" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>44.2</v>
+        <v>22.8</v>
       </c>
       <c r="H11" t="n">
-        <v>22.6</v>
+        <v>24.1</v>
       </c>
       <c r="I11" t="n">
-        <v>45.9</v>
+        <v>19.9</v>
       </c>
       <c r="J11" t="n">
-        <v>71.3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="K11" t="n">
-        <v>68.59999999999999</v>
+        <v>87.8</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1015,31 +1015,31 @@
         <v>44.9</v>
       </c>
       <c r="C12" t="n">
-        <v>53.6</v>
+        <v>32.4</v>
       </c>
       <c r="D12" t="n">
-        <v>31.1</v>
+        <v>31.8</v>
       </c>
       <c r="E12" t="n">
-        <v>78.2</v>
+        <v>62.7</v>
       </c>
       <c r="F12" t="n">
-        <v>18.4</v>
+        <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>44.2</v>
+        <v>22.7</v>
       </c>
       <c r="H12" t="n">
-        <v>70.40000000000001</v>
+        <v>70.8</v>
       </c>
       <c r="I12" t="n">
-        <v>90.5</v>
+        <v>80.7</v>
       </c>
       <c r="J12" t="n">
-        <v>45.2</v>
+        <v>15.8</v>
       </c>
       <c r="K12" t="n">
-        <v>49.7</v>
+        <v>86.2</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1065,31 +1065,31 @@
         <v>44.9</v>
       </c>
       <c r="C13" t="n">
-        <v>41.7</v>
+        <v>29.2</v>
       </c>
       <c r="D13" t="n">
-        <v>31.3</v>
+        <v>36.3</v>
       </c>
       <c r="E13" t="n">
-        <v>41.3</v>
+        <v>49.5</v>
       </c>
       <c r="F13" t="n">
-        <v>68.8</v>
+        <v>50.3</v>
       </c>
       <c r="G13" t="n">
-        <v>61.8</v>
+        <v>76.8</v>
       </c>
       <c r="H13" t="n">
-        <v>23.6</v>
+        <v>52.8</v>
       </c>
       <c r="I13" t="n">
-        <v>25.5</v>
+        <v>44.4</v>
       </c>
       <c r="J13" t="n">
-        <v>33</v>
+        <v>13.8</v>
       </c>
       <c r="K13" t="n">
-        <v>28.4</v>
+        <v>78.7</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1115,31 +1115,31 @@
         <v>44.9</v>
       </c>
       <c r="C14" t="n">
-        <v>58</v>
+        <v>75.8</v>
       </c>
       <c r="D14" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>44.3</v>
+        <v>95</v>
       </c>
       <c r="F14" t="n">
-        <v>64.8</v>
+        <v>10.6</v>
       </c>
       <c r="G14" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H14" t="n">
-        <v>27.9</v>
+        <v>58.3</v>
       </c>
       <c r="I14" t="n">
-        <v>50.8</v>
+        <v>22.1</v>
       </c>
       <c r="J14" t="n">
-        <v>67</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="K14" t="n">
-        <v>73.7</v>
+        <v>93.3</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1165,31 +1165,31 @@
         <v>44.9</v>
       </c>
       <c r="C15" t="n">
-        <v>82.7</v>
+        <v>81</v>
       </c>
       <c r="D15" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>66.40000000000001</v>
+        <v>60.4</v>
       </c>
       <c r="F15" t="n">
-        <v>72.90000000000001</v>
+        <v>42.2</v>
       </c>
       <c r="G15" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H15" t="n">
-        <v>95</v>
+        <v>91.5</v>
       </c>
       <c r="I15" t="n">
-        <v>88.90000000000001</v>
+        <v>20.7</v>
       </c>
       <c r="J15" t="n">
-        <v>33.8</v>
+        <v>27.3</v>
       </c>
       <c r="K15" t="n">
-        <v>77.59999999999999</v>
+        <v>89.5</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1215,31 +1215,31 @@
         <v>44.9</v>
       </c>
       <c r="C16" t="n">
-        <v>38.8</v>
+        <v>61.2</v>
       </c>
       <c r="D16" t="n">
         <v>95</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>38.2</v>
       </c>
       <c r="F16" t="n">
-        <v>72.2</v>
+        <v>56.4</v>
       </c>
       <c r="G16" t="n">
-        <v>11.3</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>22.5</v>
+        <v>77.2</v>
       </c>
       <c r="I16" t="n">
-        <v>12.2</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="J16" t="n">
-        <v>46.2</v>
+        <v>44.6</v>
       </c>
       <c r="K16" t="n">
-        <v>24.4</v>
+        <v>13.2</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1265,31 +1265,31 @@
         <v>44.9</v>
       </c>
       <c r="C17" t="n">
-        <v>46.6</v>
+        <v>72.5</v>
       </c>
       <c r="D17" t="n">
-        <v>31.2</v>
+        <v>73</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>16.4</v>
       </c>
       <c r="F17" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G17" t="n">
-        <v>10</v>
+        <v>41.5</v>
       </c>
       <c r="H17" t="n">
-        <v>21.7</v>
+        <v>10</v>
       </c>
       <c r="I17" t="n">
-        <v>11.5</v>
+        <v>33.7</v>
       </c>
       <c r="J17" t="n">
-        <v>36.2</v>
+        <v>64.8</v>
       </c>
       <c r="K17" t="n">
-        <v>23.8</v>
+        <v>37.3</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1315,31 +1315,31 @@
         <v>44.9</v>
       </c>
       <c r="C18" t="n">
-        <v>54.4</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="D18" t="n">
-        <v>31.1</v>
+        <v>32.6</v>
       </c>
       <c r="E18" t="n">
-        <v>61.4</v>
+        <v>58.6</v>
       </c>
       <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="H18" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="I18" t="n">
         <v>38.5</v>
-      </c>
-      <c r="G18" t="n">
-        <v>44.2</v>
-      </c>
-      <c r="H18" t="n">
-        <v>64</v>
-      </c>
-      <c r="I18" t="n">
-        <v>29.1</v>
       </c>
       <c r="J18" t="n">
         <v>95</v>
       </c>
       <c r="K18" t="n">
-        <v>35</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1365,31 +1365,31 @@
         <v>44.9</v>
       </c>
       <c r="C19" t="n">
-        <v>57.9</v>
+        <v>62.3</v>
       </c>
       <c r="D19" t="n">
-        <v>31.2</v>
+        <v>35.1</v>
       </c>
       <c r="E19" t="n">
-        <v>95</v>
+        <v>89.2</v>
       </c>
       <c r="F19" t="n">
+        <v>43.6</v>
+      </c>
+      <c r="G19" t="n">
         <v>23.5</v>
       </c>
-      <c r="G19" t="n">
-        <v>44.2</v>
-      </c>
       <c r="H19" t="n">
-        <v>90.40000000000001</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="I19" t="n">
-        <v>93.3</v>
+        <v>53.6</v>
       </c>
       <c r="J19" t="n">
-        <v>39.3</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="K19" t="n">
-        <v>61.9</v>
+        <v>61.7</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1415,31 +1415,31 @@
         <v>44.9</v>
       </c>
       <c r="C20" t="n">
-        <v>51.1</v>
+        <v>70.3</v>
       </c>
       <c r="D20" t="n">
-        <v>31.1</v>
+        <v>32.3</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>15.6</v>
       </c>
       <c r="F20" t="n">
-        <v>68.59999999999999</v>
+        <v>55.3</v>
       </c>
       <c r="G20" t="n">
-        <v>10</v>
+        <v>36.8</v>
       </c>
       <c r="H20" t="n">
-        <v>21.7</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
-        <v>11.6</v>
+        <v>32.8</v>
       </c>
       <c r="J20" t="n">
-        <v>35.6</v>
+        <v>80.3</v>
       </c>
       <c r="K20" t="n">
-        <v>23.9</v>
+        <v>10.5</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1465,31 +1465,31 @@
         <v>44.9</v>
       </c>
       <c r="C21" t="n">
-        <v>89.09999999999999</v>
+        <v>94.7</v>
       </c>
       <c r="D21" t="n">
-        <v>31.1</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>86.2</v>
+        <v>32.4</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>43.4</v>
       </c>
       <c r="G21" t="n">
-        <v>44.2</v>
+        <v>44.6</v>
       </c>
       <c r="H21" t="n">
-        <v>92.5</v>
+        <v>71.7</v>
       </c>
       <c r="I21" t="n">
-        <v>85.8</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="J21" t="n">
-        <v>34.8</v>
+        <v>63.7</v>
       </c>
       <c r="K21" t="n">
-        <v>69.09999999999999</v>
+        <v>63.7</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1515,31 +1515,31 @@
         <v>44.9</v>
       </c>
       <c r="C22" t="n">
-        <v>46.9</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="D22" t="n">
-        <v>31.1</v>
+        <v>33.5</v>
       </c>
       <c r="E22" t="n">
-        <v>43</v>
+        <v>80.5</v>
       </c>
       <c r="F22" t="n">
-        <v>62.4</v>
+        <v>10</v>
       </c>
       <c r="G22" t="n">
-        <v>44.2</v>
+        <v>44.5</v>
       </c>
       <c r="H22" t="n">
-        <v>72</v>
+        <v>63.9</v>
       </c>
       <c r="I22" t="n">
-        <v>38.6</v>
+        <v>37</v>
       </c>
       <c r="J22" t="n">
-        <v>53.9</v>
+        <v>57.7</v>
       </c>
       <c r="K22" t="n">
-        <v>42.1</v>
+        <v>45.9</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1565,31 +1565,31 @@
         <v>44.9</v>
       </c>
       <c r="C23" t="n">
-        <v>95</v>
+        <v>90.5</v>
       </c>
       <c r="D23" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>45.8</v>
+        <v>85</v>
       </c>
       <c r="F23" t="n">
-        <v>74.2</v>
+        <v>46.1</v>
       </c>
       <c r="G23" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H23" t="n">
-        <v>77</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="I23" t="n">
-        <v>55.5</v>
+        <v>21.4</v>
       </c>
       <c r="J23" t="n">
-        <v>80.40000000000001</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="K23" t="n">
-        <v>81.40000000000001</v>
+        <v>90.7</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -1615,31 +1615,31 @@
         <v>44.9</v>
       </c>
       <c r="C24" t="n">
-        <v>55.3</v>
+        <v>48.8</v>
       </c>
       <c r="D24" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>83.7</v>
+        <v>84.5</v>
       </c>
       <c r="F24" t="n">
-        <v>24.8</v>
+        <v>46.9</v>
       </c>
       <c r="G24" t="n">
-        <v>44.2</v>
+        <v>21.8</v>
       </c>
       <c r="H24" t="n">
-        <v>77.2</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="I24" t="n">
-        <v>71.5</v>
+        <v>20.9</v>
       </c>
       <c r="J24" t="n">
-        <v>46.2</v>
+        <v>37.3</v>
       </c>
       <c r="K24" t="n">
-        <v>69.09999999999999</v>
+        <v>63.7</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1665,31 +1665,31 @@
         <v>44.9</v>
       </c>
       <c r="C25" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="E25" t="n">
         <v>39.7</v>
       </c>
-      <c r="D25" t="n">
-        <v>31.1</v>
-      </c>
-      <c r="E25" t="n">
-        <v>19.8</v>
-      </c>
       <c r="F25" t="n">
-        <v>68.59999999999999</v>
+        <v>55.6</v>
       </c>
       <c r="G25" t="n">
-        <v>44.1</v>
+        <v>45.4</v>
       </c>
       <c r="H25" t="n">
-        <v>21.7</v>
+        <v>10</v>
       </c>
       <c r="I25" t="n">
-        <v>11.5</v>
+        <v>34.2</v>
       </c>
       <c r="J25" t="n">
-        <v>34.9</v>
+        <v>45.9</v>
       </c>
       <c r="K25" t="n">
-        <v>23.8</v>
+        <v>10</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -1715,31 +1715,31 @@
         <v>44.9</v>
       </c>
       <c r="C26" t="n">
-        <v>53.9</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="D26" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>44.5</v>
+        <v>26.5</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>89.7</v>
       </c>
       <c r="G26" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H26" t="n">
-        <v>45.7</v>
+        <v>36.2</v>
       </c>
       <c r="I26" t="n">
-        <v>47.6</v>
+        <v>10</v>
       </c>
       <c r="J26" t="n">
-        <v>34.8</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="K26" t="n">
-        <v>55</v>
+        <v>23.4</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -1765,31 +1765,31 @@
         <v>44.9</v>
       </c>
       <c r="C27" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D27" t="n">
-        <v>31.1</v>
+        <v>33</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>14.8</v>
       </c>
       <c r="F27" t="n">
-        <v>68.59999999999999</v>
+        <v>57.5</v>
       </c>
       <c r="G27" t="n">
-        <v>10</v>
+        <v>16.9</v>
       </c>
       <c r="H27" t="n">
-        <v>21.7</v>
+        <v>20</v>
       </c>
       <c r="I27" t="n">
-        <v>11.3</v>
+        <v>11.9</v>
       </c>
       <c r="J27" t="n">
-        <v>33.5</v>
+        <v>35.5</v>
       </c>
       <c r="K27" t="n">
-        <v>23.7</v>
+        <v>69.5</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -1815,31 +1815,31 @@
         <v>44.9</v>
       </c>
       <c r="C28" t="n">
-        <v>24.9</v>
+        <v>33.5</v>
       </c>
       <c r="D28" t="n">
-        <v>32.1</v>
+        <v>79.5</v>
       </c>
       <c r="E28" t="n">
-        <v>89.40000000000001</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="F28" t="n">
-        <v>63.5</v>
+        <v>51.2</v>
       </c>
       <c r="G28" t="n">
-        <v>44.9</v>
+        <v>74</v>
       </c>
       <c r="H28" t="n">
-        <v>27.7</v>
+        <v>30</v>
       </c>
       <c r="I28" t="n">
-        <v>49.7</v>
+        <v>95</v>
       </c>
       <c r="J28" t="n">
-        <v>34</v>
+        <v>44.9</v>
       </c>
       <c r="K28" t="n">
-        <v>62.8</v>
+        <v>61.8</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -1865,31 +1865,31 @@
         <v>44.9</v>
       </c>
       <c r="C29" t="n">
-        <v>64.3</v>
+        <v>55.1</v>
       </c>
       <c r="D29" t="n">
-        <v>78.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="E29" t="n">
-        <v>61.7</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="F29" t="n">
-        <v>61.6</v>
+        <v>10</v>
       </c>
       <c r="G29" t="n">
-        <v>73.59999999999999</v>
+        <v>76.5</v>
       </c>
       <c r="H29" t="n">
-        <v>93.3</v>
+        <v>88.2</v>
       </c>
       <c r="I29" t="n">
-        <v>36.5</v>
+        <v>70.5</v>
       </c>
       <c r="J29" t="n">
-        <v>42.8</v>
+        <v>36.1</v>
       </c>
       <c r="K29" t="n">
-        <v>45.7</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -1915,31 +1915,31 @@
         <v>44.9</v>
       </c>
       <c r="C30" t="n">
-        <v>94.8</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>31.2</v>
+        <v>34.5</v>
       </c>
       <c r="E30" t="n">
-        <v>50.8</v>
+        <v>58.2</v>
       </c>
       <c r="F30" t="n">
-        <v>42.4</v>
+        <v>43.9</v>
       </c>
       <c r="G30" t="n">
-        <v>44.2</v>
+        <v>45.5</v>
       </c>
       <c r="H30" t="n">
-        <v>48.7</v>
+        <v>63.9</v>
       </c>
       <c r="I30" t="n">
-        <v>52.3</v>
+        <v>47.7</v>
       </c>
       <c r="J30" t="n">
-        <v>63.1</v>
+        <v>77.7</v>
       </c>
       <c r="K30" t="n">
-        <v>56.1</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -1965,31 +1965,31 @@
         <v>44.9</v>
       </c>
       <c r="C31" t="n">
-        <v>94.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="D31" t="n">
-        <v>37.5</v>
+        <v>84.09999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>85.8</v>
+        <v>95</v>
       </c>
       <c r="F31" t="n">
-        <v>32.8</v>
+        <v>10</v>
       </c>
       <c r="G31" t="n">
-        <v>47.9</v>
+        <v>78</v>
       </c>
       <c r="H31" t="n">
-        <v>84.40000000000001</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="I31" t="n">
-        <v>74.3</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="J31" t="n">
-        <v>82.40000000000001</v>
+        <v>95</v>
       </c>
       <c r="K31" t="n">
-        <v>53.5</v>
+        <v>56</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2015,31 +2015,31 @@
         <v>44.9</v>
       </c>
       <c r="C32" t="n">
-        <v>75.40000000000001</v>
+        <v>95</v>
       </c>
       <c r="D32" t="n">
-        <v>93.2</v>
+        <v>84.8</v>
       </c>
       <c r="E32" t="n">
-        <v>48.8</v>
+        <v>27.1</v>
       </c>
       <c r="F32" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>88.09999999999999</v>
+        <v>81.59999999999999</v>
       </c>
       <c r="H32" t="n">
-        <v>85.3</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="I32" t="n">
-        <v>81.40000000000001</v>
+        <v>84.3</v>
       </c>
       <c r="J32" t="n">
-        <v>34.5</v>
+        <v>36.9</v>
       </c>
       <c r="K32" t="n">
-        <v>49.7</v>
+        <v>53.3</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -2065,31 +2065,31 @@
         <v>44.9</v>
       </c>
       <c r="C33" t="n">
-        <v>65.40000000000001</v>
+        <v>34</v>
       </c>
       <c r="D33" t="n">
+        <v>87.2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="F33" t="n">
+        <v>93.09999999999999</v>
+      </c>
+      <c r="G33" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="H33" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="I33" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="J33" t="n">
         <v>62.7</v>
       </c>
-      <c r="E33" t="n">
-        <v>70.2</v>
-      </c>
-      <c r="F33" t="n">
-        <v>68.59999999999999</v>
-      </c>
-      <c r="G33" t="n">
-        <v>85</v>
-      </c>
-      <c r="H33" t="n">
-        <v>61.3</v>
-      </c>
-      <c r="I33" t="n">
-        <v>33.9</v>
-      </c>
-      <c r="J33" t="n">
-        <v>43.8</v>
-      </c>
       <c r="K33" t="n">
-        <v>32.2</v>
+        <v>10</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -2115,31 +2115,31 @@
         <v>44.9</v>
       </c>
       <c r="C34" t="n">
-        <v>39</v>
+        <v>43.7</v>
       </c>
       <c r="D34" t="n">
-        <v>31.1</v>
+        <v>33</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>14.2</v>
       </c>
       <c r="F34" t="n">
-        <v>68.59999999999999</v>
+        <v>55.9</v>
       </c>
       <c r="G34" t="n">
-        <v>10</v>
+        <v>18.7</v>
       </c>
       <c r="H34" t="n">
-        <v>22</v>
+        <v>45.4</v>
       </c>
       <c r="I34" t="n">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="J34" t="n">
-        <v>38.9</v>
+        <v>45.3</v>
       </c>
       <c r="K34" t="n">
-        <v>23.7</v>
+        <v>11.8</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2165,31 +2165,31 @@
         <v>44.9</v>
       </c>
       <c r="C35" t="n">
-        <v>94</v>
+        <v>89.7</v>
       </c>
       <c r="D35" t="n">
-        <v>33.2</v>
+        <v>40.6</v>
       </c>
       <c r="E35" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F35" t="n">
-        <v>10</v>
+        <v>37.4</v>
       </c>
       <c r="G35" t="n">
-        <v>46.2</v>
+        <v>54.2</v>
       </c>
       <c r="H35" t="n">
-        <v>95</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="I35" t="n">
-        <v>93.8</v>
+        <v>86.7</v>
       </c>
       <c r="J35" t="n">
-        <v>34.5</v>
+        <v>46.1</v>
       </c>
       <c r="K35" t="n">
-        <v>82.40000000000001</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
@@ -2215,31 +2215,31 @@
         <v>44.9</v>
       </c>
       <c r="C36" t="n">
-        <v>37.7</v>
+        <v>10</v>
       </c>
       <c r="D36" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
       </c>
       <c r="F36" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G36" t="n">
-        <v>10</v>
+        <v>16.4</v>
       </c>
       <c r="H36" t="n">
-        <v>21.7</v>
+        <v>20.5</v>
       </c>
       <c r="I36" t="n">
         <v>11.4</v>
       </c>
       <c r="J36" t="n">
-        <v>33.3</v>
+        <v>27.3</v>
       </c>
       <c r="K36" t="n">
-        <v>23.7</v>
+        <v>11.8</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
@@ -2265,31 +2265,31 @@
         <v>44.9</v>
       </c>
       <c r="C37" t="n">
-        <v>50.1</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>31.1</v>
+        <v>31.4</v>
       </c>
       <c r="E37" t="n">
-        <v>36.7</v>
+        <v>49.2</v>
       </c>
       <c r="F37" t="n">
-        <v>52.3</v>
+        <v>42.3</v>
       </c>
       <c r="G37" t="n">
-        <v>34.3</v>
+        <v>43.1</v>
       </c>
       <c r="H37" t="n">
-        <v>55.4</v>
+        <v>69.5</v>
       </c>
       <c r="I37" t="n">
-        <v>31.9</v>
+        <v>45.2</v>
       </c>
       <c r="J37" t="n">
-        <v>38.7</v>
+        <v>54.4</v>
       </c>
       <c r="K37" t="n">
-        <v>34.6</v>
+        <v>45.2</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2315,31 +2315,31 @@
         <v>44.9</v>
       </c>
       <c r="C38" t="n">
-        <v>47.3</v>
+        <v>50.3</v>
       </c>
       <c r="D38" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>55.4</v>
+        <v>29.8</v>
       </c>
       <c r="F38" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G38" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H38" t="n">
-        <v>53.2</v>
+        <v>90.7</v>
       </c>
       <c r="I38" t="n">
-        <v>24.3</v>
+        <v>10</v>
       </c>
       <c r="J38" t="n">
         <v>95</v>
       </c>
       <c r="K38" t="n">
-        <v>33.5</v>
+        <v>49.4</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2365,31 +2365,31 @@
         <v>44.9</v>
       </c>
       <c r="C39" t="n">
-        <v>53.8</v>
+        <v>66.8</v>
       </c>
       <c r="D39" t="n">
-        <v>31.1</v>
+        <v>33.1</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>15.3</v>
       </c>
       <c r="F39" t="n">
-        <v>68.59999999999999</v>
+        <v>51.1</v>
       </c>
       <c r="G39" t="n">
-        <v>10</v>
+        <v>17.3</v>
       </c>
       <c r="H39" t="n">
-        <v>35.8</v>
+        <v>80.2</v>
       </c>
       <c r="I39" t="n">
-        <v>11.8</v>
+        <v>12.1</v>
       </c>
       <c r="J39" t="n">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="K39" t="n">
-        <v>24.3</v>
+        <v>40.9</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
@@ -2415,31 +2415,31 @@
         <v>44.9</v>
       </c>
       <c r="C40" t="n">
-        <v>42</v>
+        <v>63.1</v>
       </c>
       <c r="D40" t="n">
-        <v>95</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="E40" t="n">
-        <v>41.2</v>
+        <v>22.1</v>
       </c>
       <c r="F40" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G40" t="n">
-        <v>95</v>
+        <v>81.7</v>
       </c>
       <c r="H40" t="n">
-        <v>25.1</v>
+        <v>51.4</v>
       </c>
       <c r="I40" t="n">
-        <v>91.59999999999999</v>
+        <v>84</v>
       </c>
       <c r="J40" t="n">
-        <v>33.6</v>
+        <v>27.7</v>
       </c>
       <c r="K40" t="n">
-        <v>45.1</v>
+        <v>43.3</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
@@ -2465,31 +2465,31 @@
         <v>95</v>
       </c>
       <c r="C41" t="n">
-        <v>46.1</v>
+        <v>31.9</v>
       </c>
       <c r="D41" t="n">
-        <v>31.2</v>
+        <v>74.3</v>
       </c>
       <c r="E41" t="n">
-        <v>42.6</v>
+        <v>79.3</v>
       </c>
       <c r="F41" t="n">
-        <v>63.5</v>
+        <v>10</v>
       </c>
       <c r="G41" t="n">
-        <v>44.3</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>23.7</v>
+        <v>58.2</v>
       </c>
       <c r="I41" t="n">
-        <v>45.4</v>
+        <v>77.7</v>
       </c>
       <c r="J41" t="n">
-        <v>33</v>
+        <v>13.7</v>
       </c>
       <c r="K41" t="n">
-        <v>45.9</v>
+        <v>54.1</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
@@ -2515,31 +2515,31 @@
         <v>44.9</v>
       </c>
       <c r="C42" t="n">
-        <v>37.8</v>
+        <v>10.1</v>
       </c>
       <c r="D42" t="n">
-        <v>87.3</v>
+        <v>85</v>
       </c>
       <c r="E42" t="n">
-        <v>41.1</v>
+        <v>21.3</v>
       </c>
       <c r="F42" t="n">
-        <v>68.59999999999999</v>
+        <v>59.3</v>
       </c>
       <c r="G42" t="n">
         <v>95</v>
       </c>
       <c r="H42" t="n">
-        <v>26.3</v>
+        <v>10</v>
       </c>
       <c r="I42" t="n">
-        <v>80.40000000000001</v>
+        <v>80.2</v>
       </c>
       <c r="J42" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="K42" t="n">
-        <v>39</v>
+        <v>11.1</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
@@ -2565,31 +2565,31 @@
         <v>44.9</v>
       </c>
       <c r="C43" t="n">
-        <v>74.2</v>
+        <v>31.7</v>
       </c>
       <c r="D43" t="n">
-        <v>31.3</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>41.5</v>
+        <v>24.4</v>
       </c>
       <c r="F43" t="n">
-        <v>68.5</v>
+        <v>52.3</v>
       </c>
       <c r="G43" t="n">
-        <v>44.5</v>
+        <v>89.8</v>
       </c>
       <c r="H43" t="n">
-        <v>22.2</v>
+        <v>25.9</v>
       </c>
       <c r="I43" t="n">
-        <v>45.3</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="J43" t="n">
-        <v>45.4</v>
+        <v>27.9</v>
       </c>
       <c r="K43" t="n">
-        <v>46.5</v>
+        <v>57.1</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -2615,31 +2615,31 @@
         <v>44.9</v>
       </c>
       <c r="C44" t="n">
-        <v>43.3</v>
+        <v>34</v>
       </c>
       <c r="D44" t="n">
-        <v>95</v>
+        <v>83.5</v>
       </c>
       <c r="E44" t="n">
-        <v>54.9</v>
+        <v>52.8</v>
       </c>
       <c r="F44" t="n">
-        <v>68.59999999999999</v>
+        <v>60.2</v>
       </c>
       <c r="G44" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H44" t="n">
-        <v>21.7</v>
+        <v>19.7</v>
       </c>
       <c r="I44" t="n">
-        <v>95</v>
+        <v>83.2</v>
       </c>
       <c r="J44" t="n">
-        <v>33.1</v>
+        <v>19.1</v>
       </c>
       <c r="K44" t="n">
-        <v>45.3</v>
+        <v>15</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -2665,31 +2665,31 @@
         <v>44.9</v>
       </c>
       <c r="C45" t="n">
-        <v>63.9</v>
+        <v>84</v>
       </c>
       <c r="D45" t="n">
-        <v>31.6</v>
+        <v>80.5</v>
       </c>
       <c r="E45" t="n">
-        <v>51.1</v>
+        <v>59.1</v>
       </c>
       <c r="F45" t="n">
-        <v>95</v>
+        <v>42.7</v>
       </c>
       <c r="G45" t="n">
-        <v>44.9</v>
+        <v>91.7</v>
       </c>
       <c r="H45" t="n">
-        <v>78.3</v>
+        <v>71.3</v>
       </c>
       <c r="I45" t="n">
-        <v>47.4</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="J45" t="n">
-        <v>33.1</v>
+        <v>14.5</v>
       </c>
       <c r="K45" t="n">
-        <v>61.1</v>
+        <v>24.2</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -2715,31 +2715,31 @@
         <v>44.9</v>
       </c>
       <c r="C46" t="n">
-        <v>64.8</v>
+        <v>38.1</v>
       </c>
       <c r="D46" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E46" t="n">
-        <v>84.90000000000001</v>
+        <v>62.7</v>
       </c>
       <c r="F46" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G46" t="n">
-        <v>44.2</v>
+        <v>10</v>
       </c>
       <c r="H46" t="n">
-        <v>93.5</v>
+        <v>73.09999999999999</v>
       </c>
       <c r="I46" t="n">
-        <v>76.2</v>
+        <v>23.6</v>
       </c>
       <c r="J46" t="n">
-        <v>45.6</v>
+        <v>27.2</v>
       </c>
       <c r="K46" t="n">
-        <v>64.5</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -2765,31 +2765,31 @@
         <v>44.9</v>
       </c>
       <c r="C47" t="n">
-        <v>67.5</v>
+        <v>42.7</v>
       </c>
       <c r="D47" t="n">
-        <v>31.1</v>
+        <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>18.1</v>
       </c>
       <c r="F47" t="n">
-        <v>65.8</v>
+        <v>45.5</v>
       </c>
       <c r="G47" t="n">
         <v>10</v>
       </c>
       <c r="H47" t="n">
-        <v>32.1</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="I47" t="n">
-        <v>13.1</v>
+        <v>10</v>
       </c>
       <c r="J47" t="n">
-        <v>33.8</v>
+        <v>27.7</v>
       </c>
       <c r="K47" t="n">
-        <v>29.3</v>
+        <v>79</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -2815,31 +2815,31 @@
         <v>44.9</v>
       </c>
       <c r="C48" t="n">
-        <v>53.3</v>
+        <v>94.2</v>
       </c>
       <c r="D48" t="n">
-        <v>31.1</v>
+        <v>73</v>
       </c>
       <c r="E48" t="n">
-        <v>77.59999999999999</v>
+        <v>84.3</v>
       </c>
       <c r="F48" t="n">
-        <v>61.9</v>
+        <v>43.9</v>
       </c>
       <c r="G48" t="n">
-        <v>44.2</v>
+        <v>68.8</v>
       </c>
       <c r="H48" t="n">
-        <v>89.2</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="I48" t="n">
+        <v>94.5</v>
+      </c>
+      <c r="J48" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="K48" t="n">
         <v>95</v>
-      </c>
-      <c r="J48" t="n">
-        <v>34</v>
-      </c>
-      <c r="K48" t="n">
-        <v>82.59999999999999</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -2865,31 +2865,31 @@
         <v>44.9</v>
       </c>
       <c r="C49" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D49" t="n">
-        <v>31.1</v>
+        <v>33</v>
       </c>
       <c r="E49" t="n">
-        <v>10</v>
+        <v>15.7</v>
       </c>
       <c r="F49" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="G49" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="H49" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="I49" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="J49" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="K49" t="n">
         <v>68.59999999999999</v>
-      </c>
-      <c r="G49" t="n">
-        <v>10</v>
-      </c>
-      <c r="H49" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="I49" t="n">
-        <v>11.4</v>
-      </c>
-      <c r="J49" t="n">
-        <v>35.3</v>
-      </c>
-      <c r="K49" t="n">
-        <v>23.8</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -2915,31 +2915,31 @@
         <v>44.9</v>
       </c>
       <c r="C50" t="n">
-        <v>31.8</v>
+        <v>70.2</v>
       </c>
       <c r="D50" t="n">
-        <v>48</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="E50" t="n">
-        <v>93.59999999999999</v>
+        <v>91.8</v>
       </c>
       <c r="F50" t="n">
-        <v>28.7</v>
+        <v>47</v>
       </c>
       <c r="G50" t="n">
-        <v>57.7</v>
+        <v>85.59999999999999</v>
       </c>
       <c r="H50" t="n">
-        <v>49.1</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="I50" t="n">
-        <v>61.2</v>
+        <v>95</v>
       </c>
       <c r="J50" t="n">
-        <v>35.7</v>
+        <v>56</v>
       </c>
       <c r="K50" t="n">
-        <v>51.8</v>
+        <v>55.7</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -2965,31 +2965,31 @@
         <v>44.9</v>
       </c>
       <c r="C51" t="n">
-        <v>37.8</v>
+        <v>21.2</v>
       </c>
       <c r="D51" t="n">
-        <v>31.1</v>
+        <v>33.3</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>14.9</v>
       </c>
       <c r="F51" t="n">
-        <v>68.59999999999999</v>
+        <v>93.09999999999999</v>
       </c>
       <c r="G51" t="n">
-        <v>10</v>
+        <v>17.8</v>
       </c>
       <c r="H51" t="n">
-        <v>21.6</v>
+        <v>20.1</v>
       </c>
       <c r="I51" t="n">
-        <v>11.6</v>
+        <v>32.4</v>
       </c>
       <c r="J51" t="n">
-        <v>33.1</v>
+        <v>14</v>
       </c>
       <c r="K51" t="n">
-        <v>23.7</v>
+        <v>36.3</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -3015,31 +3015,31 @@
         <v>44.9</v>
       </c>
       <c r="C52" t="n">
-        <v>45.6</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>95</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="E52" t="n">
-        <v>25.5</v>
+        <v>15.5</v>
       </c>
       <c r="F52" t="n">
-        <v>68.59999999999999</v>
+        <v>58</v>
       </c>
       <c r="G52" t="n">
-        <v>74</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H52" t="n">
-        <v>21.7</v>
+        <v>20.3</v>
       </c>
       <c r="I52" t="n">
-        <v>68.90000000000001</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="J52" t="n">
-        <v>38.3</v>
+        <v>72.7</v>
       </c>
       <c r="K52" t="n">
-        <v>37.3</v>
+        <v>71.2</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
@@ -3065,31 +3065,31 @@
         <v>44.9</v>
       </c>
       <c r="C53" t="n">
-        <v>54.5</v>
+        <v>70.7</v>
       </c>
       <c r="D53" t="n">
-        <v>31.2</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="E53" t="n">
-        <v>67.8</v>
+        <v>59.5</v>
       </c>
       <c r="F53" t="n">
-        <v>35.8</v>
+        <v>40.3</v>
       </c>
       <c r="G53" t="n">
-        <v>44.2</v>
+        <v>69</v>
       </c>
       <c r="H53" t="n">
-        <v>69.09999999999999</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="I53" t="n">
-        <v>53.8</v>
+        <v>76.3</v>
       </c>
       <c r="J53" t="n">
-        <v>35.1</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="K53" t="n">
-        <v>77.2</v>
+        <v>65.5</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
@@ -3115,31 +3115,31 @@
         <v>44.9</v>
       </c>
       <c r="C54" t="n">
-        <v>80.40000000000001</v>
+        <v>81.59999999999999</v>
       </c>
       <c r="D54" t="n">
-        <v>31.3</v>
+        <v>77</v>
       </c>
       <c r="E54" t="n">
-        <v>41.5</v>
+        <v>22.9</v>
       </c>
       <c r="F54" t="n">
-        <v>10</v>
+        <v>37.8</v>
       </c>
       <c r="G54" t="n">
-        <v>44.4</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="H54" t="n">
-        <v>43</v>
+        <v>34.8</v>
       </c>
       <c r="I54" t="n">
-        <v>11.4</v>
+        <v>46.3</v>
       </c>
       <c r="J54" t="n">
-        <v>61.8</v>
+        <v>88.8</v>
       </c>
       <c r="K54" t="n">
-        <v>25.7</v>
+        <v>20.9</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -3165,31 +3165,31 @@
         <v>44.9</v>
       </c>
       <c r="C55" t="n">
-        <v>39.5</v>
+        <v>22.2</v>
       </c>
       <c r="D55" t="n">
-        <v>31.1</v>
+        <v>32.8</v>
       </c>
       <c r="E55" t="n">
-        <v>41.2</v>
+        <v>20.6</v>
       </c>
       <c r="F55" t="n">
-        <v>68.8</v>
+        <v>91.8</v>
       </c>
       <c r="G55" t="n">
-        <v>89</v>
+        <v>52.4</v>
       </c>
       <c r="H55" t="n">
-        <v>21.6</v>
+        <v>18.6</v>
       </c>
       <c r="I55" t="n">
-        <v>11.4</v>
+        <v>31.7</v>
       </c>
       <c r="J55" t="n">
-        <v>33.9</v>
+        <v>62.8</v>
       </c>
       <c r="K55" t="n">
-        <v>23.7</v>
+        <v>35.4</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
@@ -3215,31 +3215,31 @@
         <v>44.9</v>
       </c>
       <c r="C56" t="n">
-        <v>38.6</v>
+        <v>22.9</v>
       </c>
       <c r="D56" t="n">
-        <v>95</v>
+        <v>83.2</v>
       </c>
       <c r="E56" t="n">
-        <v>41.3</v>
+        <v>49.3</v>
       </c>
       <c r="F56" t="n">
-        <v>68.3</v>
+        <v>56.9</v>
       </c>
       <c r="G56" t="n">
-        <v>95</v>
+        <v>82.8</v>
       </c>
       <c r="H56" t="n">
-        <v>21.7</v>
+        <v>18.3</v>
       </c>
       <c r="I56" t="n">
-        <v>95</v>
+        <v>83.2</v>
       </c>
       <c r="J56" t="n">
-        <v>33.4</v>
+        <v>35.5</v>
       </c>
       <c r="K56" t="n">
-        <v>45.2</v>
+        <v>10</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
@@ -3265,31 +3265,31 @@
         <v>44.9</v>
       </c>
       <c r="C57" t="n">
-        <v>44.7</v>
+        <v>51.6</v>
       </c>
       <c r="D57" t="n">
-        <v>95</v>
+        <v>87.2</v>
       </c>
       <c r="E57" t="n">
-        <v>86.90000000000001</v>
+        <v>53.4</v>
       </c>
       <c r="F57" t="n">
-        <v>46.2</v>
+        <v>48.2</v>
       </c>
       <c r="G57" t="n">
-        <v>93.3</v>
+        <v>84</v>
       </c>
       <c r="H57" t="n">
-        <v>27.4</v>
+        <v>22.7</v>
       </c>
       <c r="I57" t="n">
-        <v>77.3</v>
+        <v>82.7</v>
       </c>
       <c r="J57" t="n">
-        <v>46.2</v>
+        <v>45</v>
       </c>
       <c r="K57" t="n">
-        <v>38.9</v>
+        <v>36.8</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update the phenotype-microbiomeand statistic etc
</commit_message>
<xml_diff>
--- a/output/vaginal_probability_sample_estimation.xlsx
+++ b/output/vaginal_probability_sample_estimation.xlsx
@@ -16,34 +16,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
   <si>
-    <t>pelvic inflammatory diseases</t>
-  </si>
-  <si>
-    <t>endometritis</t>
-  </si>
-  <si>
-    <t>miscarriage</t>
-  </si>
-  <si>
-    <t>ovarian cancer</t>
-  </si>
-  <si>
-    <t>Cervical intraepithelial neoplasia</t>
-  </si>
-  <si>
-    <t>preterm prelabor rupture of membranes (PPROM)</t>
-  </si>
-  <si>
-    <t>dysmenorrhea(Menstrual pain)</t>
-  </si>
-  <si>
-    <t>adenomyosis</t>
-  </si>
-  <si>
-    <t>vaginal dryness</t>
-  </si>
-  <si>
-    <t>gestational diabetes</t>
+    <t>Pelvic Inflammatory Diseases</t>
+  </si>
+  <si>
+    <t>Endometritis</t>
+  </si>
+  <si>
+    <t>Miscarriage</t>
+  </si>
+  <si>
+    <t>Ovarian Cancer</t>
+  </si>
+  <si>
+    <t>Cervical Intraepithelial Neoplasia</t>
+  </si>
+  <si>
+    <t>Preterm Prelabor Rupture of Membranes (PPROM)</t>
+  </si>
+  <si>
+    <t>Dysmenorrhea (Menstrual pain)</t>
+  </si>
+  <si>
+    <t>Adenomyosis</t>
+  </si>
+  <si>
+    <t>Vaginal Dryness</t>
+  </si>
+  <si>
+    <t>Gestational Diabetes</t>
   </si>
   <si>
     <t>subCST</t>
@@ -681,7 +681,7 @@
         <v>44.9</v>
       </c>
       <c r="C2">
-        <v>40.7</v>
+        <v>37.4</v>
       </c>
       <c r="D2">
         <v>86.40000000000001</v>
@@ -725,7 +725,7 @@
         <v>44.9</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>6.7</v>
       </c>
       <c r="D3">
         <v>47.4</v>
@@ -769,7 +769,7 @@
         <v>44.9</v>
       </c>
       <c r="C4">
-        <v>49.8</v>
+        <v>61.5</v>
       </c>
       <c r="D4">
         <v>74.90000000000001</v>
@@ -813,7 +813,7 @@
         <v>44.9</v>
       </c>
       <c r="C5">
-        <v>67.09999999999999</v>
+        <v>66.3</v>
       </c>
       <c r="D5">
         <v>6.5</v>
@@ -901,7 +901,7 @@
         <v>44.9</v>
       </c>
       <c r="C7">
-        <v>13.1</v>
+        <v>10.4</v>
       </c>
       <c r="D7">
         <v>31.5</v>
@@ -945,7 +945,7 @@
         <v>44.9</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="D8">
         <v>40.8</v>
@@ -989,7 +989,7 @@
         <v>44.9</v>
       </c>
       <c r="C9">
-        <v>16.7</v>
+        <v>23.4</v>
       </c>
       <c r="D9">
         <v>76.59999999999999</v>
@@ -1077,7 +1077,7 @@
         <v>44.9</v>
       </c>
       <c r="C11">
-        <v>7.9</v>
+        <v>5.9</v>
       </c>
       <c r="D11">
         <v>31.9</v>
@@ -1121,7 +1121,7 @@
         <v>44.9</v>
       </c>
       <c r="C12">
-        <v>32.4</v>
+        <v>42.7</v>
       </c>
       <c r="D12">
         <v>31.8</v>
@@ -1165,7 +1165,7 @@
         <v>44.9</v>
       </c>
       <c r="C13">
-        <v>29.2</v>
+        <v>38.9</v>
       </c>
       <c r="D13">
         <v>36.3</v>
@@ -1209,7 +1209,7 @@
         <v>44.9</v>
       </c>
       <c r="C14">
-        <v>75.8</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="D14">
         <v>6.5</v>
@@ -1253,7 +1253,7 @@
         <v>44.9</v>
       </c>
       <c r="C15">
-        <v>81</v>
+        <v>80.3</v>
       </c>
       <c r="D15">
         <v>6.5</v>
@@ -1297,7 +1297,7 @@
         <v>44.9</v>
       </c>
       <c r="C16">
-        <v>61.2</v>
+        <v>60.7</v>
       </c>
       <c r="D16">
         <v>95</v>
@@ -1341,7 +1341,7 @@
         <v>44.9</v>
       </c>
       <c r="C17">
-        <v>72.5</v>
+        <v>72.2</v>
       </c>
       <c r="D17">
         <v>73</v>
@@ -1385,7 +1385,7 @@
         <v>44.9</v>
       </c>
       <c r="C18">
-        <v>83.59999999999999</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="D18">
         <v>32.6</v>
@@ -1429,7 +1429,7 @@
         <v>44.9</v>
       </c>
       <c r="C19">
-        <v>62.3</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>35.1</v>
@@ -1473,7 +1473,7 @@
         <v>44.9</v>
       </c>
       <c r="C20">
-        <v>70.3</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="D20">
         <v>32.3</v>
@@ -1517,7 +1517,7 @@
         <v>44.9</v>
       </c>
       <c r="C21">
-        <v>94.7</v>
+        <v>95</v>
       </c>
       <c r="D21">
         <v>71.59999999999999</v>
@@ -1561,7 +1561,7 @@
         <v>44.9</v>
       </c>
       <c r="C22">
-        <v>87.09999999999999</v>
+        <v>87.2</v>
       </c>
       <c r="D22">
         <v>33.5</v>
@@ -1605,7 +1605,7 @@
         <v>44.9</v>
       </c>
       <c r="C23">
-        <v>90.5</v>
+        <v>89.8</v>
       </c>
       <c r="D23">
         <v>6.5</v>
@@ -1649,7 +1649,7 @@
         <v>44.9</v>
       </c>
       <c r="C24">
-        <v>48.8</v>
+        <v>44.9</v>
       </c>
       <c r="D24">
         <v>6.5</v>
@@ -1693,7 +1693,7 @@
         <v>44.9</v>
       </c>
       <c r="C25">
-        <v>22.5</v>
+        <v>19.9</v>
       </c>
       <c r="D25">
         <v>33.7</v>
@@ -1737,7 +1737,7 @@
         <v>44.9</v>
       </c>
       <c r="C26">
-        <v>69.09999999999999</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="D26">
         <v>6.5</v>
@@ -1781,7 +1781,7 @@
         <v>44.9</v>
       </c>
       <c r="C27">
-        <v>8.300000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="D27">
         <v>33</v>
@@ -1825,7 +1825,7 @@
         <v>44.9</v>
       </c>
       <c r="C28">
-        <v>33.5</v>
+        <v>30.8</v>
       </c>
       <c r="D28">
         <v>79.5</v>
@@ -1869,7 +1869,7 @@
         <v>44.9</v>
       </c>
       <c r="C29">
-        <v>55.1</v>
+        <v>54.2</v>
       </c>
       <c r="D29">
         <v>95</v>
@@ -1913,7 +1913,7 @@
         <v>44.9</v>
       </c>
       <c r="C30">
-        <v>76.09999999999999</v>
+        <v>74.5</v>
       </c>
       <c r="D30">
         <v>34.5</v>
@@ -2045,7 +2045,7 @@
         <v>44.9</v>
       </c>
       <c r="C33">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D33">
         <v>87.2</v>
@@ -2089,7 +2089,7 @@
         <v>44.9</v>
       </c>
       <c r="C34">
-        <v>43.7</v>
+        <v>42.1</v>
       </c>
       <c r="D34">
         <v>33</v>
@@ -2133,7 +2133,7 @@
         <v>44.9</v>
       </c>
       <c r="C35">
-        <v>89.7</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="D35">
         <v>40.6</v>
@@ -2221,7 +2221,7 @@
         <v>44.9</v>
       </c>
       <c r="C37">
-        <v>69.90000000000001</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="D37">
         <v>31.4</v>
@@ -2265,7 +2265,7 @@
         <v>44.9</v>
       </c>
       <c r="C38">
-        <v>50.3</v>
+        <v>47.2</v>
       </c>
       <c r="D38">
         <v>6.5</v>
@@ -2309,7 +2309,7 @@
         <v>44.9</v>
       </c>
       <c r="C39">
-        <v>66.8</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="D39">
         <v>33.1</v>
@@ -2353,7 +2353,7 @@
         <v>44.9</v>
       </c>
       <c r="C40">
-        <v>63.1</v>
+        <v>62.2</v>
       </c>
       <c r="D40">
         <v>84.59999999999999</v>
@@ -2397,7 +2397,7 @@
         <v>95</v>
       </c>
       <c r="C41">
-        <v>31.9</v>
+        <v>25.5</v>
       </c>
       <c r="D41">
         <v>74.3</v>
@@ -2441,7 +2441,7 @@
         <v>44.9</v>
       </c>
       <c r="C42">
-        <v>10.1</v>
+        <v>7.9</v>
       </c>
       <c r="D42">
         <v>85</v>
@@ -2485,7 +2485,7 @@
         <v>44.9</v>
       </c>
       <c r="C43">
-        <v>31.7</v>
+        <v>25.2</v>
       </c>
       <c r="D43">
         <v>77.59999999999999</v>
@@ -2529,7 +2529,7 @@
         <v>44.9</v>
       </c>
       <c r="C44">
-        <v>34</v>
+        <v>30.5</v>
       </c>
       <c r="D44">
         <v>83.5</v>
@@ -2573,7 +2573,7 @@
         <v>44.9</v>
       </c>
       <c r="C45">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45">
         <v>80.5</v>
@@ -2617,7 +2617,7 @@
         <v>44.9</v>
       </c>
       <c r="C46">
-        <v>38.1</v>
+        <v>33.1</v>
       </c>
       <c r="D46">
         <v>6.5</v>
@@ -2661,7 +2661,7 @@
         <v>44.9</v>
       </c>
       <c r="C47">
-        <v>42.7</v>
+        <v>54.1</v>
       </c>
       <c r="D47">
         <v>6.5</v>
@@ -2705,7 +2705,7 @@
         <v>44.9</v>
       </c>
       <c r="C48">
-        <v>94.2</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="D48">
         <v>73</v>
@@ -2749,7 +2749,7 @@
         <v>44.9</v>
       </c>
       <c r="C49">
-        <v>46</v>
+        <v>42.7</v>
       </c>
       <c r="D49">
         <v>33</v>
@@ -2793,7 +2793,7 @@
         <v>44.9</v>
       </c>
       <c r="C50">
-        <v>70.2</v>
+        <v>70.3</v>
       </c>
       <c r="D50">
         <v>87.59999999999999</v>
@@ -2837,7 +2837,7 @@
         <v>44.9</v>
       </c>
       <c r="C51">
-        <v>21.2</v>
+        <v>29.2</v>
       </c>
       <c r="D51">
         <v>33.3</v>
@@ -2881,7 +2881,7 @@
         <v>44.9</v>
       </c>
       <c r="C52">
-        <v>25</v>
+        <v>22.9</v>
       </c>
       <c r="D52">
         <v>82.59999999999999</v>
@@ -2925,7 +2925,7 @@
         <v>44.9</v>
       </c>
       <c r="C53">
-        <v>70.7</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="D53">
         <v>74.40000000000001</v>
@@ -2969,7 +2969,7 @@
         <v>44.9</v>
       </c>
       <c r="C54">
-        <v>81.59999999999999</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="D54">
         <v>77</v>
@@ -3013,7 +3013,7 @@
         <v>44.9</v>
       </c>
       <c r="C55">
-        <v>22.2</v>
+        <v>20.2</v>
       </c>
       <c r="D55">
         <v>32.8</v>
@@ -3057,7 +3057,7 @@
         <v>44.9</v>
       </c>
       <c r="C56">
-        <v>22.9</v>
+        <v>31.3</v>
       </c>
       <c r="D56">
         <v>83.2</v>
@@ -3101,7 +3101,7 @@
         <v>44.9</v>
       </c>
       <c r="C57">
-        <v>51.6</v>
+        <v>50.8</v>
       </c>
       <c r="D57">
         <v>87.2</v>

</xml_diff>

<commit_message>
New code - percentile_rank
</commit_message>
<xml_diff>
--- a/output/vaginal_probability_sample_estimation.xlsx
+++ b/output/vaginal_probability_sample_estimation.xlsx
@@ -678,34 +678,34 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>37.4</v>
+        <v>37.5</v>
       </c>
       <c r="D2">
-        <v>86.40000000000001</v>
+        <v>89.3</v>
       </c>
       <c r="E2">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F2">
-        <v>63.5</v>
+        <v>58</v>
       </c>
       <c r="G2">
-        <v>23.7</v>
+        <v>29.5</v>
       </c>
       <c r="H2">
-        <v>53.5</v>
+        <v>54.5</v>
       </c>
       <c r="I2">
-        <v>60.8</v>
+        <v>75</v>
       </c>
       <c r="J2">
-        <v>48.2</v>
+        <v>44.6</v>
       </c>
       <c r="K2">
-        <v>88.8</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="L2" t="s">
         <v>70</v>
@@ -722,34 +722,34 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>6.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="D3">
-        <v>47.4</v>
+        <v>54.5</v>
       </c>
       <c r="E3">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F3">
-        <v>30.5</v>
+        <v>32.1</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
       <c r="H3">
-        <v>24.7</v>
+        <v>29.5</v>
       </c>
       <c r="I3">
-        <v>53.3</v>
+        <v>46.4</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="K3">
-        <v>44.3</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>71</v>
@@ -766,34 +766,34 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>61.5</v>
+        <v>57.1</v>
       </c>
       <c r="D4">
-        <v>74.90000000000001</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="E4">
-        <v>57.1</v>
+        <v>70.5</v>
       </c>
       <c r="F4">
-        <v>46.9</v>
+        <v>50.9</v>
       </c>
       <c r="G4">
-        <v>81.09999999999999</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="H4">
-        <v>37.3</v>
+        <v>44.6</v>
       </c>
       <c r="I4">
-        <v>58.6</v>
+        <v>65.2</v>
       </c>
       <c r="J4">
-        <v>78.40000000000001</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="K4">
-        <v>6.8</v>
+        <v>5</v>
       </c>
       <c r="L4" t="s">
         <v>70</v>
@@ -810,34 +810,34 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>66.3</v>
+        <v>64.3</v>
       </c>
       <c r="D5">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>42</v>
+        <v>27.7</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
       <c r="G5">
-        <v>32.1</v>
+        <v>39.3</v>
       </c>
       <c r="H5">
         <v>5</v>
       </c>
       <c r="I5">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J5">
-        <v>25.4</v>
+        <v>28.6</v>
       </c>
       <c r="K5">
-        <v>89.2</v>
+        <v>90.2</v>
       </c>
       <c r="L5" t="s">
         <v>72</v>
@@ -854,34 +854,34 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>19.6</v>
       </c>
       <c r="E6">
+        <v>58</v>
+      </c>
+      <c r="F6">
         <v>54.5</v>
       </c>
-      <c r="F6">
-        <v>52.6</v>
-      </c>
       <c r="G6">
-        <v>18</v>
+        <v>10.7</v>
       </c>
       <c r="H6">
-        <v>9.9</v>
+        <v>8.9</v>
       </c>
       <c r="I6">
-        <v>22</v>
+        <v>16.1</v>
       </c>
       <c r="J6">
-        <v>69.59999999999999</v>
+        <v>70.5</v>
       </c>
       <c r="K6">
-        <v>22.2</v>
+        <v>21.4</v>
       </c>
       <c r="L6" t="s">
         <v>73</v>
@@ -898,34 +898,34 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>10.4</v>
+        <v>12.5</v>
       </c>
       <c r="D7">
-        <v>31.5</v>
+        <v>21.4</v>
       </c>
       <c r="E7">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F7">
-        <v>44.7</v>
+        <v>46.4</v>
       </c>
       <c r="G7">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="H7">
-        <v>19.3</v>
+        <v>17</v>
       </c>
       <c r="I7">
-        <v>58.8</v>
+        <v>70.5</v>
       </c>
       <c r="J7">
-        <v>25.1</v>
+        <v>25</v>
       </c>
       <c r="K7">
-        <v>73.2</v>
+        <v>75</v>
       </c>
       <c r="L7" t="s">
         <v>74</v>
@@ -942,31 +942,31 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="D8">
-        <v>40.8</v>
+        <v>52.7</v>
       </c>
       <c r="E8">
-        <v>41.7</v>
+        <v>25.9</v>
       </c>
       <c r="F8">
-        <v>72.90000000000001</v>
+        <v>67</v>
       </c>
       <c r="G8">
-        <v>70</v>
+        <v>63.4</v>
       </c>
       <c r="H8">
-        <v>82.90000000000001</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="I8">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J8">
-        <v>70.8</v>
+        <v>72.3</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -986,34 +986,34 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>23.4</v>
+        <v>20.5</v>
       </c>
       <c r="D9">
-        <v>76.59999999999999</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="E9">
-        <v>9.4</v>
+        <v>17</v>
       </c>
       <c r="F9">
-        <v>90.8</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="G9">
-        <v>58.9</v>
+        <v>53.6</v>
       </c>
       <c r="H9">
-        <v>83.09999999999999</v>
+        <v>81.2</v>
       </c>
       <c r="I9">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J9">
-        <v>19.5</v>
+        <v>19.6</v>
       </c>
       <c r="K9">
-        <v>65.3</v>
+        <v>58</v>
       </c>
       <c r="L9" t="s">
         <v>75</v>
@@ -1030,34 +1030,34 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>70.7</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="D10">
-        <v>83.09999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="E10">
-        <v>89.8</v>
+        <v>81.2</v>
       </c>
       <c r="F10">
-        <v>94.5</v>
+        <v>95</v>
       </c>
       <c r="G10">
-        <v>88.3</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="H10">
-        <v>85.7</v>
+        <v>92</v>
       </c>
       <c r="I10">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J10">
-        <v>49.1</v>
+        <v>45.5</v>
       </c>
       <c r="K10">
-        <v>66.09999999999999</v>
+        <v>62.5</v>
       </c>
       <c r="L10" t="s">
         <v>71</v>
@@ -1074,34 +1074,34 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>5.9</v>
+        <v>7.1</v>
       </c>
       <c r="D11">
-        <v>31.9</v>
+        <v>26.8</v>
       </c>
       <c r="E11">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F11">
-        <v>22.8</v>
+        <v>26.8</v>
       </c>
       <c r="G11">
-        <v>24.1</v>
+        <v>30.4</v>
       </c>
       <c r="H11">
-        <v>19.9</v>
+        <v>19.6</v>
       </c>
       <c r="I11">
-        <v>58.6</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="J11">
-        <v>87.8</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="K11">
-        <v>48.8</v>
+        <v>53.6</v>
       </c>
       <c r="L11" t="s">
         <v>74</v>
@@ -1118,34 +1118,34 @@
         <v>24</v>
       </c>
       <c r="B12">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>42.7</v>
+        <v>42</v>
       </c>
       <c r="D12">
-        <v>31.8</v>
+        <v>24.1</v>
       </c>
       <c r="E12">
-        <v>5.9</v>
+        <v>6.2</v>
       </c>
       <c r="F12">
-        <v>22.7</v>
+        <v>25.9</v>
       </c>
       <c r="G12">
-        <v>70.8</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="H12">
-        <v>80.7</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="I12">
-        <v>32.1</v>
+        <v>34.8</v>
       </c>
       <c r="J12">
-        <v>86.2</v>
+        <v>84.8</v>
       </c>
       <c r="K12">
-        <v>18.1</v>
+        <v>14.3</v>
       </c>
       <c r="L12" t="s">
         <v>74</v>
@@ -1162,34 +1162,34 @@
         <v>25</v>
       </c>
       <c r="B13">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>38.9</v>
+        <v>39.3</v>
       </c>
       <c r="D13">
-        <v>36.3</v>
+        <v>48.2</v>
       </c>
       <c r="E13">
-        <v>50.3</v>
+        <v>50.9</v>
       </c>
       <c r="F13">
-        <v>76.8</v>
+        <v>73.2</v>
       </c>
       <c r="G13">
-        <v>52.8</v>
+        <v>46.4</v>
       </c>
       <c r="H13">
-        <v>44.4</v>
+        <v>47.3</v>
       </c>
       <c r="I13">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J13">
-        <v>78.7</v>
+        <v>77.7</v>
       </c>
       <c r="K13">
-        <v>18.1</v>
+        <v>17.9</v>
       </c>
       <c r="L13" t="s">
         <v>73</v>
@@ -1206,34 +1206,34 @@
         <v>26</v>
       </c>
       <c r="B14">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>74.90000000000001</v>
+        <v>79.5</v>
       </c>
       <c r="D14">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>10.6</v>
+        <v>18.8</v>
       </c>
       <c r="F14">
-        <v>8.800000000000001</v>
+        <v>10.7</v>
       </c>
       <c r="G14">
-        <v>58.3</v>
+        <v>50</v>
       </c>
       <c r="H14">
-        <v>22.1</v>
+        <v>25.9</v>
       </c>
       <c r="I14">
-        <v>58.8</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="J14">
-        <v>93.3</v>
+        <v>95</v>
       </c>
       <c r="K14">
-        <v>16.7</v>
+        <v>12.5</v>
       </c>
       <c r="L14" t="s">
         <v>74</v>
@@ -1250,34 +1250,34 @@
         <v>27</v>
       </c>
       <c r="B15">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>80.3</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="D15">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>42.2</v>
+        <v>29.5</v>
       </c>
       <c r="F15">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="G15">
-        <v>91.5</v>
+        <v>95</v>
       </c>
       <c r="H15">
-        <v>20.7</v>
+        <v>20.5</v>
       </c>
       <c r="I15">
-        <v>23</v>
+        <v>28.6</v>
       </c>
       <c r="J15">
-        <v>89.5</v>
+        <v>90.2</v>
       </c>
       <c r="K15">
-        <v>30.1</v>
+        <v>28.6</v>
       </c>
       <c r="L15" t="s">
         <v>74</v>
@@ -1294,34 +1294,34 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>60.7</v>
+        <v>57.1</v>
       </c>
       <c r="D16">
         <v>95</v>
       </c>
       <c r="E16">
-        <v>56.4</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>70.40000000000001</v>
+        <v>63.4</v>
       </c>
       <c r="G16">
-        <v>77.2</v>
+        <v>76.8</v>
       </c>
       <c r="H16">
-        <v>67.40000000000001</v>
+        <v>58.9</v>
       </c>
       <c r="I16">
-        <v>22.2</v>
+        <v>18.8</v>
       </c>
       <c r="J16">
-        <v>13.2</v>
+        <v>16.1</v>
       </c>
       <c r="K16">
-        <v>40.8</v>
+        <v>39.3</v>
       </c>
       <c r="L16" t="s">
         <v>76</v>
@@ -1338,34 +1338,34 @@
         <v>29</v>
       </c>
       <c r="B17">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>72.2</v>
+        <v>75</v>
       </c>
       <c r="D17">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E17">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F17">
-        <v>41.5</v>
+        <v>35.7</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>7.1</v>
       </c>
       <c r="H17">
-        <v>33.7</v>
+        <v>37.5</v>
       </c>
       <c r="I17">
-        <v>82</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="J17">
-        <v>37.3</v>
+        <v>35.7</v>
       </c>
       <c r="K17">
-        <v>43.8</v>
+        <v>46.4</v>
       </c>
       <c r="L17" t="s">
         <v>76</v>
@@ -1382,34 +1382,34 @@
         <v>30</v>
       </c>
       <c r="B18">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>83.09999999999999</v>
+        <v>87.5</v>
       </c>
       <c r="D18">
-        <v>32.6</v>
+        <v>29.5</v>
       </c>
       <c r="E18">
-        <v>6.8</v>
+        <v>11.6</v>
       </c>
       <c r="F18">
-        <v>43.2</v>
+        <v>39.3</v>
       </c>
       <c r="G18">
-        <v>91.3</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="H18">
-        <v>38.5</v>
+        <v>45.5</v>
       </c>
       <c r="I18">
-        <v>62.4</v>
+        <v>76.8</v>
       </c>
       <c r="J18">
+        <v>81.2</v>
+      </c>
+      <c r="K18">
         <v>80.40000000000001</v>
-      </c>
-      <c r="K18">
-        <v>84.2</v>
       </c>
       <c r="L18" t="s">
         <v>77</v>
@@ -1426,34 +1426,34 @@
         <v>31</v>
       </c>
       <c r="B19">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>60</v>
+        <v>53.6</v>
       </c>
       <c r="D19">
-        <v>35.1</v>
+        <v>48.2</v>
       </c>
       <c r="E19">
-        <v>43.6</v>
+        <v>36.6</v>
       </c>
       <c r="F19">
-        <v>23.5</v>
+        <v>28.6</v>
       </c>
       <c r="G19">
-        <v>72.59999999999999</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="H19">
-        <v>53.6</v>
+        <v>55.4</v>
       </c>
       <c r="I19">
-        <v>53.1</v>
+        <v>41.1</v>
       </c>
       <c r="J19">
-        <v>61.7</v>
+        <v>58</v>
       </c>
       <c r="K19">
-        <v>32.8</v>
+        <v>30.4</v>
       </c>
       <c r="L19" t="s">
         <v>74</v>
@@ -1470,34 +1470,34 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>69.40000000000001</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="D20">
-        <v>32.3</v>
+        <v>27.7</v>
       </c>
       <c r="E20">
-        <v>55.3</v>
+        <v>59.8</v>
       </c>
       <c r="F20">
-        <v>36.8</v>
+        <v>34.8</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>21.4</v>
       </c>
       <c r="H20">
-        <v>32.8</v>
+        <v>36.6</v>
       </c>
       <c r="I20">
-        <v>95</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="J20">
-        <v>10.5</v>
+        <v>8</v>
       </c>
       <c r="K20">
-        <v>70.3</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="L20" t="s">
         <v>76</v>
@@ -1514,34 +1514,34 @@
         <v>33</v>
       </c>
       <c r="B21">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>95</v>
       </c>
       <c r="D21">
-        <v>71.59999999999999</v>
+        <v>56.2</v>
       </c>
       <c r="E21">
-        <v>43.4</v>
+        <v>34.8</v>
       </c>
       <c r="F21">
         <v>44.6</v>
       </c>
       <c r="G21">
-        <v>71.7</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="H21">
-        <v>77.90000000000001</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="I21">
-        <v>52.9</v>
+        <v>39.3</v>
       </c>
       <c r="J21">
-        <v>63.7</v>
+        <v>63.4</v>
       </c>
       <c r="K21">
-        <v>30.5</v>
+        <v>30.4</v>
       </c>
       <c r="L21" t="s">
         <v>78</v>
@@ -1558,34 +1558,34 @@
         <v>34</v>
       </c>
       <c r="B22">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>87.2</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="D22">
-        <v>33.5</v>
+        <v>41.1</v>
       </c>
       <c r="E22">
-        <v>6.5</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="F22">
-        <v>44.5</v>
+        <v>42.9</v>
       </c>
       <c r="G22">
-        <v>63.9</v>
+        <v>53.6</v>
       </c>
       <c r="H22">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I22">
-        <v>56.5</v>
+        <v>61.6</v>
       </c>
       <c r="J22">
-        <v>45.9</v>
+        <v>42</v>
       </c>
       <c r="K22">
-        <v>88.90000000000001</v>
+        <v>85.7</v>
       </c>
       <c r="L22" t="s">
         <v>72</v>
@@ -1602,34 +1602,34 @@
         <v>35</v>
       </c>
       <c r="B23">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>89.8</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="D23">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>46.1</v>
+        <v>43.8</v>
       </c>
       <c r="F23">
-        <v>8.300000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="G23">
-        <v>87.40000000000001</v>
+        <v>85.7</v>
       </c>
       <c r="H23">
-        <v>21.4</v>
+        <v>25</v>
       </c>
       <c r="I23">
-        <v>56.4</v>
+        <v>60.7</v>
       </c>
       <c r="J23">
-        <v>90.7</v>
+        <v>95</v>
       </c>
       <c r="K23">
-        <v>13.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="L23" t="s">
         <v>74</v>
@@ -1646,34 +1646,34 @@
         <v>36</v>
       </c>
       <c r="B24">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>44.9</v>
+        <v>45.5</v>
       </c>
       <c r="D24">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>46.9</v>
+        <v>45.5</v>
       </c>
       <c r="F24">
-        <v>21.8</v>
+        <v>24.1</v>
       </c>
       <c r="G24">
-        <v>68.90000000000001</v>
+        <v>58.9</v>
       </c>
       <c r="H24">
-        <v>20.9</v>
+        <v>21.4</v>
       </c>
       <c r="I24">
-        <v>22.4</v>
+        <v>25.9</v>
       </c>
       <c r="J24">
-        <v>63.7</v>
+        <v>61.6</v>
       </c>
       <c r="K24">
-        <v>51.9</v>
+        <v>57.1</v>
       </c>
       <c r="L24" t="s">
         <v>74</v>
@@ -1690,28 +1690,28 @@
         <v>37</v>
       </c>
       <c r="B25">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>19.9</v>
+        <v>14.3</v>
       </c>
       <c r="D25">
-        <v>33.7</v>
+        <v>42.9</v>
       </c>
       <c r="E25">
-        <v>55.6</v>
+        <v>63.4</v>
       </c>
       <c r="F25">
-        <v>45.4</v>
+        <v>48.2</v>
       </c>
       <c r="G25">
         <v>5</v>
       </c>
       <c r="H25">
-        <v>34.2</v>
+        <v>41.1</v>
       </c>
       <c r="I25">
-        <v>54.3</v>
+        <v>55.4</v>
       </c>
       <c r="J25">
         <v>5</v>
@@ -1734,34 +1734,34 @@
         <v>38</v>
       </c>
       <c r="B26">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>68.90000000000001</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="D26">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>89.7</v>
+        <v>79.5</v>
       </c>
       <c r="F26">
-        <v>9.1</v>
+        <v>14.3</v>
       </c>
       <c r="G26">
-        <v>36.2</v>
+        <v>42</v>
       </c>
       <c r="H26">
-        <v>5.4</v>
+        <v>7.1</v>
       </c>
       <c r="I26">
-        <v>95</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="J26">
-        <v>23.4</v>
+        <v>23.2</v>
       </c>
       <c r="K26">
-        <v>95</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="L26" t="s">
         <v>74</v>
@@ -1778,34 +1778,34 @@
         <v>39</v>
       </c>
       <c r="B27">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>6.4</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>33</v>
+        <v>33.9</v>
       </c>
       <c r="E27">
-        <v>57.5</v>
+        <v>72.3</v>
       </c>
       <c r="F27">
-        <v>16.9</v>
+        <v>17</v>
       </c>
       <c r="G27">
-        <v>20</v>
+        <v>18.8</v>
       </c>
       <c r="H27">
-        <v>11.9</v>
+        <v>13.4</v>
       </c>
       <c r="I27">
-        <v>52</v>
+        <v>35.7</v>
       </c>
       <c r="J27">
-        <v>69.5</v>
+        <v>68.8</v>
       </c>
       <c r="K27">
-        <v>68.5</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="L27" t="s">
         <v>76</v>
@@ -1822,34 +1822,34 @@
         <v>40</v>
       </c>
       <c r="B28">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>30.8</v>
+        <v>29.5</v>
       </c>
       <c r="D28">
-        <v>79.5</v>
+        <v>72.3</v>
       </c>
       <c r="E28">
-        <v>51.2</v>
+        <v>54.5</v>
       </c>
       <c r="F28">
-        <v>74</v>
+        <v>70.5</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>35.7</v>
       </c>
       <c r="H28">
         <v>95</v>
       </c>
       <c r="I28">
-        <v>81.09999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="J28">
-        <v>61.8</v>
+        <v>59.8</v>
       </c>
       <c r="K28">
-        <v>36.2</v>
+        <v>35.7</v>
       </c>
       <c r="L28" t="s">
         <v>74</v>
@@ -1866,34 +1866,34 @@
         <v>41</v>
       </c>
       <c r="B29">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>54.2</v>
+        <v>53.6</v>
       </c>
       <c r="D29">
         <v>95</v>
       </c>
       <c r="E29">
-        <v>7.6</v>
+        <v>15.2</v>
       </c>
       <c r="F29">
-        <v>76.5</v>
+        <v>73.2</v>
       </c>
       <c r="G29">
-        <v>88.2</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="H29">
-        <v>70.5</v>
+        <v>58.9</v>
       </c>
       <c r="I29">
-        <v>81.3</v>
+        <v>81.2</v>
       </c>
       <c r="J29">
-        <v>83.09999999999999</v>
+        <v>83</v>
       </c>
       <c r="K29">
-        <v>47.8</v>
+        <v>53.6</v>
       </c>
       <c r="L29" t="s">
         <v>70</v>
@@ -1910,34 +1910,34 @@
         <v>42</v>
       </c>
       <c r="B30">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>74.5</v>
+        <v>77.7</v>
       </c>
       <c r="D30">
-        <v>34.5</v>
+        <v>44.6</v>
       </c>
       <c r="E30">
-        <v>43.9</v>
+        <v>40.2</v>
       </c>
       <c r="F30">
-        <v>45.5</v>
+        <v>50</v>
       </c>
       <c r="G30">
-        <v>63.9</v>
+        <v>57.1</v>
       </c>
       <c r="H30">
-        <v>47.7</v>
+        <v>51.8</v>
       </c>
       <c r="I30">
-        <v>59.3</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="J30">
-        <v>89.40000000000001</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="K30">
-        <v>39.1</v>
+        <v>37.5</v>
       </c>
       <c r="L30" t="s">
         <v>74</v>
@@ -1954,34 +1954,34 @@
         <v>43</v>
       </c>
       <c r="B31">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>95</v>
       </c>
       <c r="D31">
-        <v>84.09999999999999</v>
+        <v>83</v>
       </c>
       <c r="E31">
-        <v>5.3</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>78</v>
+        <v>76.8</v>
       </c>
       <c r="G31">
-        <v>72.90000000000001</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H31">
-        <v>84.90000000000001</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="I31">
         <v>95</v>
       </c>
       <c r="J31">
-        <v>56</v>
+        <v>55.4</v>
       </c>
       <c r="K31">
-        <v>86.3</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="L31" t="s">
         <v>74</v>
@@ -1998,34 +1998,34 @@
         <v>44</v>
       </c>
       <c r="B32">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>95</v>
       </c>
       <c r="D32">
-        <v>84.8</v>
+        <v>85.7</v>
       </c>
       <c r="E32">
         <v>5</v>
       </c>
       <c r="F32">
-        <v>81.59999999999999</v>
+        <v>77.7</v>
       </c>
       <c r="G32">
-        <v>90.90000000000001</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="H32">
-        <v>84.3</v>
+        <v>87.5</v>
       </c>
       <c r="I32">
-        <v>53.4</v>
+        <v>46.4</v>
       </c>
       <c r="J32">
-        <v>53.3</v>
+        <v>49.1</v>
       </c>
       <c r="K32">
-        <v>65.90000000000001</v>
+        <v>58.9</v>
       </c>
       <c r="L32" t="s">
         <v>74</v>
@@ -2042,34 +2042,34 @@
         <v>45</v>
       </c>
       <c r="B33">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C33">
-        <v>31</v>
+        <v>30.4</v>
       </c>
       <c r="D33">
-        <v>87.2</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="E33">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F33">
-        <v>83.8</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="G33">
-        <v>30.5</v>
+        <v>37.5</v>
       </c>
       <c r="H33">
-        <v>76.59999999999999</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="I33">
-        <v>52.3</v>
+        <v>38.4</v>
       </c>
       <c r="J33">
         <v>5</v>
       </c>
       <c r="K33">
-        <v>89.3</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="L33" t="s">
         <v>70</v>
@@ -2086,34 +2086,34 @@
         <v>46</v>
       </c>
       <c r="B34">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>42.1</v>
+        <v>41.1</v>
       </c>
       <c r="D34">
-        <v>33</v>
+        <v>35.7</v>
       </c>
       <c r="E34">
-        <v>55.9</v>
+        <v>65.2</v>
       </c>
       <c r="F34">
-        <v>18.7</v>
+        <v>23.2</v>
       </c>
       <c r="G34">
-        <v>45.4</v>
+        <v>44.6</v>
       </c>
       <c r="H34">
-        <v>11.4</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="I34">
-        <v>23.6</v>
+        <v>32.1</v>
       </c>
       <c r="J34">
-        <v>11.8</v>
+        <v>11.6</v>
       </c>
       <c r="K34">
-        <v>68.90000000000001</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="L34" t="s">
         <v>76</v>
@@ -2130,34 +2130,34 @@
         <v>47</v>
       </c>
       <c r="B35">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>90.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="D35">
-        <v>40.6</v>
+        <v>50.9</v>
       </c>
       <c r="E35">
-        <v>37.4</v>
+        <v>20.5</v>
       </c>
       <c r="F35">
-        <v>54.2</v>
+        <v>56.2</v>
       </c>
       <c r="G35">
-        <v>93.09999999999999</v>
+        <v>95</v>
       </c>
       <c r="H35">
-        <v>86.7</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="I35">
-        <v>55.7</v>
+        <v>55.4</v>
       </c>
       <c r="J35">
-        <v>90.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="K35">
-        <v>28.1</v>
+        <v>26.8</v>
       </c>
       <c r="L35" t="s">
         <v>74</v>
@@ -2174,34 +2174,34 @@
         <v>48</v>
       </c>
       <c r="B36">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C36">
         <v>5</v>
       </c>
       <c r="D36">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F36">
-        <v>16.4</v>
+        <v>14.3</v>
       </c>
       <c r="G36">
-        <v>20.5</v>
+        <v>25.9</v>
       </c>
       <c r="H36">
-        <v>11.4</v>
+        <v>12.5</v>
       </c>
       <c r="I36">
-        <v>22.3</v>
+        <v>19.6</v>
       </c>
       <c r="J36">
-        <v>11.8</v>
+        <v>12.5</v>
       </c>
       <c r="K36">
-        <v>68</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="L36" t="s">
         <v>76</v>
@@ -2218,34 +2218,34 @@
         <v>49</v>
       </c>
       <c r="B37">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <v>69.40000000000001</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="D37">
-        <v>31.4</v>
+        <v>21.4</v>
       </c>
       <c r="E37">
-        <v>42.3</v>
+        <v>31.2</v>
       </c>
       <c r="F37">
-        <v>43.1</v>
+        <v>37.5</v>
       </c>
       <c r="G37">
-        <v>69.5</v>
+        <v>61.6</v>
       </c>
       <c r="H37">
-        <v>45.2</v>
+        <v>49.1</v>
       </c>
       <c r="I37">
-        <v>53.1</v>
+        <v>42.9</v>
       </c>
       <c r="J37">
-        <v>45.2</v>
+        <v>41.1</v>
       </c>
       <c r="K37">
-        <v>18.3</v>
+        <v>18.8</v>
       </c>
       <c r="L37" t="s">
         <v>72</v>
@@ -2262,22 +2262,22 @@
         <v>50</v>
       </c>
       <c r="B38">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>47.2</v>
+        <v>46.4</v>
       </c>
       <c r="D38">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>6.9</v>
+        <v>13.4</v>
       </c>
       <c r="F38">
-        <v>8.199999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="G38">
-        <v>90.7</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="H38">
         <v>5</v>
@@ -2286,7 +2286,7 @@
         <v>95</v>
       </c>
       <c r="J38">
-        <v>49.4</v>
+        <v>48.2</v>
       </c>
       <c r="K38">
         <v>95</v>
@@ -2306,34 +2306,34 @@
         <v>51</v>
       </c>
       <c r="B39">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>65.09999999999999</v>
+        <v>60.7</v>
       </c>
       <c r="D39">
-        <v>33.1</v>
+        <v>39.3</v>
       </c>
       <c r="E39">
-        <v>51.1</v>
+        <v>52.7</v>
       </c>
       <c r="F39">
-        <v>17.3</v>
+        <v>19.6</v>
       </c>
       <c r="G39">
-        <v>80.2</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H39">
-        <v>12.1</v>
+        <v>15.2</v>
       </c>
       <c r="I39">
-        <v>56.5</v>
+        <v>63.4</v>
       </c>
       <c r="J39">
-        <v>40.9</v>
+        <v>36.6</v>
       </c>
       <c r="K39">
-        <v>88.90000000000001</v>
+        <v>87.5</v>
       </c>
       <c r="L39" t="s">
         <v>76</v>
@@ -2350,34 +2350,34 @@
         <v>52</v>
       </c>
       <c r="B40">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>62.2</v>
+        <v>59.8</v>
       </c>
       <c r="D40">
-        <v>84.59999999999999</v>
+        <v>85.7</v>
       </c>
       <c r="E40">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F40">
-        <v>81.7</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="G40">
-        <v>51.4</v>
+        <v>45.5</v>
       </c>
       <c r="H40">
-        <v>84</v>
+        <v>87.5</v>
       </c>
       <c r="I40">
-        <v>22.9</v>
+        <v>27.7</v>
       </c>
       <c r="J40">
-        <v>43.3</v>
+        <v>37.5</v>
       </c>
       <c r="K40">
-        <v>45.4</v>
+        <v>50.9</v>
       </c>
       <c r="L40" t="s">
         <v>74</v>
@@ -2397,31 +2397,31 @@
         <v>95</v>
       </c>
       <c r="C41">
-        <v>25.5</v>
+        <v>25</v>
       </c>
       <c r="D41">
-        <v>74.3</v>
+        <v>62.5</v>
       </c>
       <c r="E41">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="F41">
-        <v>87.59999999999999</v>
+        <v>89.3</v>
       </c>
       <c r="G41">
-        <v>58.2</v>
+        <v>50</v>
       </c>
       <c r="H41">
-        <v>77.7</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="I41">
-        <v>21.8</v>
+        <v>15.2</v>
       </c>
       <c r="J41">
-        <v>54.1</v>
+        <v>50</v>
       </c>
       <c r="K41">
-        <v>26.1</v>
+        <v>23.2</v>
       </c>
       <c r="L41" t="s">
         <v>74</v>
@@ -2438,34 +2438,34 @@
         <v>54</v>
       </c>
       <c r="B42">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>7.9</v>
+        <v>12.5</v>
       </c>
       <c r="D42">
-        <v>85</v>
+        <v>89.3</v>
       </c>
       <c r="E42">
-        <v>59.3</v>
+        <v>76.8</v>
       </c>
       <c r="F42">
         <v>95</v>
       </c>
       <c r="G42">
-        <v>5.9</v>
+        <v>5</v>
       </c>
       <c r="H42">
-        <v>80.2</v>
+        <v>72.3</v>
       </c>
       <c r="I42">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J42">
-        <v>11.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="K42">
-        <v>43.9</v>
+        <v>46.4</v>
       </c>
       <c r="L42" t="s">
         <v>70</v>
@@ -2482,34 +2482,34 @@
         <v>55</v>
       </c>
       <c r="B43">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C43">
-        <v>25.2</v>
+        <v>21.4</v>
       </c>
       <c r="D43">
-        <v>77.59999999999999</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="E43">
-        <v>52.3</v>
+        <v>55.4</v>
       </c>
       <c r="F43">
-        <v>89.8</v>
+        <v>90.2</v>
       </c>
       <c r="G43">
-        <v>25.9</v>
+        <v>33.9</v>
       </c>
       <c r="H43">
-        <v>79.09999999999999</v>
+        <v>70.5</v>
       </c>
       <c r="I43">
-        <v>56</v>
+        <v>57.1</v>
       </c>
       <c r="J43">
-        <v>57.1</v>
+        <v>55.4</v>
       </c>
       <c r="K43">
-        <v>74.90000000000001</v>
+        <v>76.8</v>
       </c>
       <c r="L43" t="s">
         <v>79</v>
@@ -2526,34 +2526,34 @@
         <v>56</v>
       </c>
       <c r="B44">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C44">
-        <v>30.5</v>
+        <v>27.7</v>
       </c>
       <c r="D44">
-        <v>83.5</v>
+        <v>81.2</v>
       </c>
       <c r="E44">
-        <v>60.2</v>
+        <v>76.8</v>
       </c>
       <c r="F44">
-        <v>93</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="G44">
-        <v>19.7</v>
+        <v>17.9</v>
       </c>
       <c r="H44">
-        <v>83.2</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="I44">
-        <v>21.5</v>
+        <v>13.4</v>
       </c>
       <c r="J44">
-        <v>15</v>
+        <v>17.9</v>
       </c>
       <c r="K44">
-        <v>68.40000000000001</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="L44" t="s">
         <v>71</v>
@@ -2570,34 +2570,34 @@
         <v>57</v>
       </c>
       <c r="B45">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>83</v>
+        <v>84.8</v>
       </c>
       <c r="D45">
-        <v>80.5</v>
+        <v>75</v>
       </c>
       <c r="E45">
-        <v>42.7</v>
+        <v>33</v>
       </c>
       <c r="F45">
-        <v>91.7</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="G45">
-        <v>71.3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="H45">
-        <v>82.59999999999999</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="I45">
-        <v>25.5</v>
+        <v>33.9</v>
       </c>
       <c r="J45">
-        <v>24.2</v>
+        <v>25</v>
       </c>
       <c r="K45">
-        <v>90</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="L45" t="s">
         <v>72</v>
@@ -2614,34 +2614,34 @@
         <v>58</v>
       </c>
       <c r="B46">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>33.1</v>
+        <v>33.9</v>
       </c>
       <c r="D46">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E46">
         <v>5</v>
       </c>
       <c r="F46">
-        <v>8.800000000000001</v>
+        <v>10.7</v>
       </c>
       <c r="G46">
-        <v>73.09999999999999</v>
+        <v>73.2</v>
       </c>
       <c r="H46">
-        <v>23.6</v>
+        <v>27.7</v>
       </c>
       <c r="I46">
-        <v>53.5</v>
+        <v>48.2</v>
       </c>
       <c r="J46">
-        <v>90.40000000000001</v>
+        <v>93.8</v>
       </c>
       <c r="K46">
-        <v>35.7</v>
+        <v>32.1</v>
       </c>
       <c r="L46" t="s">
         <v>74</v>
@@ -2658,31 +2658,31 @@
         <v>59</v>
       </c>
       <c r="B47">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>54.1</v>
+        <v>50.9</v>
       </c>
       <c r="D47">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E47">
-        <v>45.5</v>
+        <v>42</v>
       </c>
       <c r="F47">
         <v>5</v>
       </c>
       <c r="G47">
-        <v>83.59999999999999</v>
+        <v>81.2</v>
       </c>
       <c r="H47">
         <v>5</v>
       </c>
       <c r="I47">
-        <v>22.3</v>
+        <v>21.4</v>
       </c>
       <c r="J47">
-        <v>79</v>
+        <v>79.5</v>
       </c>
       <c r="K47">
         <v>5</v>
@@ -2702,34 +2702,34 @@
         <v>60</v>
       </c>
       <c r="B48">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>94.09999999999999</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="D48">
-        <v>73</v>
+        <v>59.8</v>
       </c>
       <c r="E48">
-        <v>43.9</v>
+        <v>37.5</v>
       </c>
       <c r="F48">
-        <v>68.8</v>
+        <v>59.8</v>
       </c>
       <c r="G48">
-        <v>88.90000000000001</v>
+        <v>90.2</v>
       </c>
       <c r="H48">
-        <v>94.5</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="I48">
-        <v>53.5</v>
+        <v>51.8</v>
       </c>
       <c r="J48">
         <v>95</v>
       </c>
       <c r="K48">
-        <v>8.300000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="L48" t="s">
         <v>74</v>
@@ -2746,34 +2746,34 @@
         <v>61</v>
       </c>
       <c r="B49">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C49">
-        <v>42.7</v>
+        <v>42.9</v>
       </c>
       <c r="D49">
-        <v>33</v>
+        <v>37.5</v>
       </c>
       <c r="E49">
-        <v>55.5</v>
+        <v>61.6</v>
       </c>
       <c r="F49">
-        <v>36.5</v>
+        <v>33.9</v>
       </c>
       <c r="G49">
-        <v>18.9</v>
+        <v>16.1</v>
       </c>
       <c r="H49">
-        <v>32.7</v>
+        <v>34.8</v>
       </c>
       <c r="I49">
-        <v>83.09999999999999</v>
+        <v>85.7</v>
       </c>
       <c r="J49">
-        <v>68.59999999999999</v>
+        <v>67</v>
       </c>
       <c r="K49">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L49" t="s">
         <v>76</v>
@@ -2790,34 +2790,34 @@
         <v>62</v>
       </c>
       <c r="B50">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C50">
-        <v>70.3</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="D50">
-        <v>87.59999999999999</v>
+        <v>95</v>
       </c>
       <c r="E50">
-        <v>47</v>
+        <v>48.2</v>
       </c>
       <c r="F50">
-        <v>85.59999999999999</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="G50">
-        <v>87.09999999999999</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="H50">
         <v>95</v>
       </c>
       <c r="I50">
-        <v>83.59999999999999</v>
+        <v>90.2</v>
       </c>
       <c r="J50">
-        <v>55.7</v>
+        <v>51.8</v>
       </c>
       <c r="K50">
-        <v>14.8</v>
+        <v>10.7</v>
       </c>
       <c r="L50" t="s">
         <v>74</v>
@@ -2834,34 +2834,34 @@
         <v>63</v>
       </c>
       <c r="B51">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>29.2</v>
+        <v>26.8</v>
       </c>
       <c r="D51">
-        <v>33.3</v>
+        <v>39.3</v>
       </c>
       <c r="E51">
-        <v>93.09999999999999</v>
+        <v>92</v>
       </c>
       <c r="F51">
-        <v>17.8</v>
+        <v>21.4</v>
       </c>
       <c r="G51">
-        <v>20.1</v>
+        <v>22.3</v>
       </c>
       <c r="H51">
-        <v>32.4</v>
+        <v>32.1</v>
       </c>
       <c r="I51">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="J51">
-        <v>36.3</v>
+        <v>31.2</v>
       </c>
       <c r="K51">
-        <v>21.5</v>
+        <v>19.6</v>
       </c>
       <c r="L51" t="s">
         <v>76</v>
@@ -2878,34 +2878,34 @@
         <v>64</v>
       </c>
       <c r="B52">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>22.9</v>
+        <v>18.8</v>
       </c>
       <c r="D52">
-        <v>82.59999999999999</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="E52">
-        <v>58</v>
+        <v>73.2</v>
       </c>
       <c r="F52">
-        <v>71.40000000000001</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="G52">
-        <v>20.3</v>
+        <v>24.1</v>
       </c>
       <c r="H52">
-        <v>74.59999999999999</v>
+        <v>62.5</v>
       </c>
       <c r="I52">
-        <v>82.7</v>
+        <v>84.8</v>
       </c>
       <c r="J52">
-        <v>71.2</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="K52">
-        <v>42.8</v>
+        <v>42.9</v>
       </c>
       <c r="L52" t="s">
         <v>71</v>
@@ -2922,34 +2922,34 @@
         <v>65</v>
       </c>
       <c r="B53">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C53">
-        <v>69.40000000000001</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="D53">
-        <v>74.40000000000001</v>
+        <v>62.5</v>
       </c>
       <c r="E53">
-        <v>40.3</v>
+        <v>24.1</v>
       </c>
       <c r="F53">
-        <v>69</v>
+        <v>61.6</v>
       </c>
       <c r="G53">
-        <v>65.09999999999999</v>
+        <v>58</v>
       </c>
       <c r="H53">
-        <v>76.3</v>
+        <v>62.5</v>
       </c>
       <c r="I53">
-        <v>83.09999999999999</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="J53">
-        <v>65.5</v>
+        <v>65.2</v>
       </c>
       <c r="K53">
-        <v>10.3</v>
+        <v>8.9</v>
       </c>
       <c r="L53" t="s">
         <v>74</v>
@@ -2966,34 +2966,34 @@
         <v>66</v>
       </c>
       <c r="B54">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C54">
-        <v>82.09999999999999</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="D54">
-        <v>77</v>
+        <v>68.8</v>
       </c>
       <c r="E54">
-        <v>37.8</v>
+        <v>22.3</v>
       </c>
       <c r="F54">
-        <v>72.90000000000001</v>
+        <v>68.8</v>
       </c>
       <c r="G54">
-        <v>34.8</v>
+        <v>40.2</v>
       </c>
       <c r="H54">
-        <v>46.3</v>
+        <v>50.9</v>
       </c>
       <c r="I54">
         <v>95</v>
       </c>
       <c r="J54">
-        <v>20.9</v>
+        <v>19.6</v>
       </c>
       <c r="K54">
-        <v>66</v>
+        <v>61.6</v>
       </c>
       <c r="L54" t="s">
         <v>72</v>
@@ -3010,34 +3010,34 @@
         <v>67</v>
       </c>
       <c r="B55">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C55">
-        <v>20.2</v>
+        <v>16.1</v>
       </c>
       <c r="D55">
-        <v>32.8</v>
+        <v>32.1</v>
       </c>
       <c r="E55">
-        <v>91.8</v>
+        <v>83</v>
       </c>
       <c r="F55">
-        <v>52.4</v>
+        <v>52.7</v>
       </c>
       <c r="G55">
-        <v>18.6</v>
+        <v>14.3</v>
       </c>
       <c r="H55">
-        <v>31.7</v>
+        <v>31.2</v>
       </c>
       <c r="I55">
-        <v>80.5</v>
+        <v>76.8</v>
       </c>
       <c r="J55">
-        <v>35.4</v>
+        <v>29.5</v>
       </c>
       <c r="K55">
-        <v>42.6</v>
+        <v>42</v>
       </c>
       <c r="L55" t="s">
         <v>80</v>
@@ -3054,34 +3054,34 @@
         <v>68</v>
       </c>
       <c r="B56">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C56">
-        <v>31.3</v>
+        <v>33.9</v>
       </c>
       <c r="D56">
-        <v>83.2</v>
+        <v>79.5</v>
       </c>
       <c r="E56">
-        <v>56.9</v>
+        <v>68.8</v>
       </c>
       <c r="F56">
-        <v>82.8</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="G56">
-        <v>18.3</v>
+        <v>11.6</v>
       </c>
       <c r="H56">
-        <v>83.2</v>
+        <v>85.7</v>
       </c>
       <c r="I56">
-        <v>22.4</v>
+        <v>24.1</v>
       </c>
       <c r="J56">
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="K56">
-        <v>42.6</v>
+        <v>41.1</v>
       </c>
       <c r="L56" t="s">
         <v>71</v>
@@ -3098,34 +3098,34 @@
         <v>69</v>
       </c>
       <c r="B57">
-        <v>44.9</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>50.8</v>
+        <v>50</v>
       </c>
       <c r="D57">
-        <v>87.2</v>
+        <v>92</v>
       </c>
       <c r="E57">
-        <v>48.2</v>
+        <v>49.1</v>
       </c>
       <c r="F57">
-        <v>84</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="G57">
-        <v>22.7</v>
+        <v>27.7</v>
       </c>
       <c r="H57">
-        <v>82.7</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="I57">
-        <v>53.8</v>
+        <v>53.6</v>
       </c>
       <c r="J57">
-        <v>36.8</v>
+        <v>32.1</v>
       </c>
       <c r="K57">
-        <v>66.59999999999999</v>
+        <v>64.3</v>
       </c>
       <c r="L57" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Modify the phenotyep-microbiome - vaginal dryness & Endomentris
</commit_message>
<xml_diff>
--- a/output/vaginal_probability_sample_estimation.xlsx
+++ b/output/vaginal_probability_sample_estimation.xlsx
@@ -792,7 +792,7 @@
         <v>54.6</v>
       </c>
       <c r="E2">
-        <v>50.1</v>
+        <v>49.1</v>
       </c>
       <c r="F2">
         <v>84.8</v>
@@ -810,7 +810,7 @@
         <v>23.5</v>
       </c>
       <c r="K2">
-        <v>28.1</v>
+        <v>53.2</v>
       </c>
       <c r="L2" t="s">
         <v>105</v>
@@ -854,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="K3">
-        <v>10.4</v>
+        <v>5</v>
       </c>
       <c r="L3" t="s">
         <v>105</v>
@@ -880,7 +880,7 @@
         <v>37.4</v>
       </c>
       <c r="E4">
-        <v>47.1</v>
+        <v>44.5</v>
       </c>
       <c r="F4">
         <v>14.2</v>
@@ -898,7 +898,7 @@
         <v>82.8</v>
       </c>
       <c r="K4">
-        <v>65.90000000000001</v>
+        <v>81.5</v>
       </c>
       <c r="L4" t="s">
         <v>106</v>
@@ -924,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>50.8</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>85.3</v>
@@ -942,7 +942,7 @@
         <v>32.3</v>
       </c>
       <c r="K5">
-        <v>46.6</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
         <v>107</v>
@@ -986,7 +986,7 @@
         <v>17.7</v>
       </c>
       <c r="K6">
-        <v>58.2</v>
+        <v>73.5</v>
       </c>
       <c r="L6" t="s">
         <v>108</v>
@@ -1012,7 +1012,7 @@
         <v>18.5</v>
       </c>
       <c r="E7">
-        <v>7.2</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F7">
         <v>66.5</v>
@@ -1030,7 +1030,7 @@
         <v>5.9</v>
       </c>
       <c r="K7">
-        <v>10.9</v>
+        <v>29.7</v>
       </c>
       <c r="L7" t="s">
         <v>109</v>
@@ -1056,7 +1056,7 @@
         <v>84.90000000000001</v>
       </c>
       <c r="E8">
-        <v>7.3</v>
+        <v>8.6</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -1074,7 +1074,7 @@
         <v>71.7</v>
       </c>
       <c r="K8">
-        <v>87.09999999999999</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="L8" t="s">
         <v>109</v>
@@ -1100,7 +1100,7 @@
         <v>85.09999999999999</v>
       </c>
       <c r="E9">
-        <v>19.8</v>
+        <v>21.5</v>
       </c>
       <c r="F9">
         <v>58</v>
@@ -1118,7 +1118,7 @@
         <v>60.4</v>
       </c>
       <c r="K9">
-        <v>38.9</v>
+        <v>23.7</v>
       </c>
       <c r="L9" t="s">
         <v>110</v>
@@ -1144,7 +1144,7 @@
         <v>87.59999999999999</v>
       </c>
       <c r="E10">
-        <v>72.2</v>
+        <v>72</v>
       </c>
       <c r="F10">
         <v>58.8</v>
@@ -1162,7 +1162,7 @@
         <v>89.8</v>
       </c>
       <c r="K10">
-        <v>37.3</v>
+        <v>54.1</v>
       </c>
       <c r="L10" t="s">
         <v>105</v>
@@ -1188,7 +1188,7 @@
         <v>19.2</v>
       </c>
       <c r="E11">
-        <v>7.8</v>
+        <v>9.1</v>
       </c>
       <c r="F11">
         <v>41.2</v>
@@ -1206,7 +1206,7 @@
         <v>23.9</v>
       </c>
       <c r="K11">
-        <v>72.8</v>
+        <v>89.7</v>
       </c>
       <c r="L11" t="s">
         <v>109</v>
@@ -1232,7 +1232,7 @@
         <v>82.7</v>
       </c>
       <c r="E12">
-        <v>40.1</v>
+        <v>58.4</v>
       </c>
       <c r="F12">
         <v>13.4</v>
@@ -1250,7 +1250,7 @@
         <v>72.5</v>
       </c>
       <c r="K12">
-        <v>78.59999999999999</v>
+        <v>88.3</v>
       </c>
       <c r="L12" t="s">
         <v>109</v>
@@ -1276,7 +1276,7 @@
         <v>44.9</v>
       </c>
       <c r="E13">
-        <v>35.2</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>13.4</v>
@@ -1294,7 +1294,7 @@
         <v>54</v>
       </c>
       <c r="K13">
-        <v>68</v>
+        <v>81.7</v>
       </c>
       <c r="L13" t="s">
         <v>108</v>
@@ -1320,7 +1320,7 @@
         <v>21.4</v>
       </c>
       <c r="E14">
-        <v>75.5</v>
+        <v>77.7</v>
       </c>
       <c r="F14">
         <v>12.2</v>
@@ -1338,7 +1338,7 @@
         <v>59.7</v>
       </c>
       <c r="K14">
-        <v>82.7</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="L14" t="s">
         <v>109</v>
@@ -1364,7 +1364,7 @@
         <v>20</v>
       </c>
       <c r="E15">
-        <v>69.7</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="F15">
         <v>23.7</v>
@@ -1382,7 +1382,7 @@
         <v>92.8</v>
       </c>
       <c r="K15">
-        <v>95</v>
+        <v>91.2</v>
       </c>
       <c r="L15" t="s">
         <v>109</v>
@@ -1408,7 +1408,7 @@
         <v>69.09999999999999</v>
       </c>
       <c r="E16">
-        <v>75.2</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="F16">
         <v>33.5</v>
@@ -1426,7 +1426,7 @@
         <v>79</v>
       </c>
       <c r="K16">
-        <v>29.5</v>
+        <v>16.7</v>
       </c>
       <c r="L16" t="s">
         <v>111</v>
@@ -1452,7 +1452,7 @@
         <v>33.7</v>
       </c>
       <c r="E17">
-        <v>58.2</v>
+        <v>55.6</v>
       </c>
       <c r="F17">
         <v>36.3</v>
@@ -1470,7 +1470,7 @@
         <v>5.5</v>
       </c>
       <c r="K17">
-        <v>60.1</v>
+        <v>42.4</v>
       </c>
       <c r="L17" t="s">
         <v>111</v>
@@ -1496,7 +1496,7 @@
         <v>38.7</v>
       </c>
       <c r="E18">
-        <v>76.40000000000001</v>
+        <v>74.3</v>
       </c>
       <c r="F18">
         <v>79.2</v>
@@ -1514,7 +1514,7 @@
         <v>92.59999999999999</v>
       </c>
       <c r="K18">
-        <v>71.8</v>
+        <v>83.2</v>
       </c>
       <c r="L18" t="s">
         <v>112</v>
@@ -1540,7 +1540,7 @@
         <v>54.7</v>
       </c>
       <c r="E19">
-        <v>74.8</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="F19">
         <v>26.2</v>
@@ -1558,7 +1558,7 @@
         <v>74.40000000000001</v>
       </c>
       <c r="K19">
-        <v>81</v>
+        <v>66.2</v>
       </c>
       <c r="L19" t="s">
         <v>109</v>
@@ -1584,7 +1584,7 @@
         <v>32.7</v>
       </c>
       <c r="E20">
-        <v>70</v>
+        <v>67.5</v>
       </c>
       <c r="F20">
         <v>63.3</v>
@@ -1602,7 +1602,7 @@
         <v>19.7</v>
       </c>
       <c r="K20">
-        <v>25</v>
+        <v>13.6</v>
       </c>
       <c r="L20" t="s">
         <v>111</v>
@@ -1646,7 +1646,7 @@
         <v>73.40000000000001</v>
       </c>
       <c r="K21">
-        <v>82.40000000000001</v>
+        <v>68</v>
       </c>
       <c r="L21" t="s">
         <v>113</v>
@@ -1672,7 +1672,7 @@
         <v>37.1</v>
       </c>
       <c r="E22">
-        <v>81.8</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="F22">
         <v>84.8</v>
@@ -1690,7 +1690,7 @@
         <v>65.40000000000001</v>
       </c>
       <c r="K22">
-        <v>31.8</v>
+        <v>51</v>
       </c>
       <c r="L22" t="s">
         <v>107</v>
@@ -1716,7 +1716,7 @@
         <v>20.7</v>
       </c>
       <c r="E23">
-        <v>92.3</v>
+        <v>92.8</v>
       </c>
       <c r="F23">
         <v>9.800000000000001</v>
@@ -1734,7 +1734,7 @@
         <v>88.90000000000001</v>
       </c>
       <c r="K23">
-        <v>95</v>
+        <v>92.2</v>
       </c>
       <c r="L23" t="s">
         <v>109</v>
@@ -1760,7 +1760,7 @@
         <v>20.2</v>
       </c>
       <c r="E24">
-        <v>58.8</v>
+        <v>60.3</v>
       </c>
       <c r="F24">
         <v>44.2</v>
@@ -1778,7 +1778,7 @@
         <v>70.59999999999999</v>
       </c>
       <c r="K24">
-        <v>82.40000000000001</v>
+        <v>68</v>
       </c>
       <c r="L24" t="s">
         <v>109</v>
@@ -1804,7 +1804,7 @@
         <v>34.1</v>
       </c>
       <c r="E25">
-        <v>16.4</v>
+        <v>15</v>
       </c>
       <c r="F25">
         <v>94.3</v>
@@ -1822,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="K25">
-        <v>6.2</v>
+        <v>5</v>
       </c>
       <c r="L25" t="s">
         <v>106</v>
@@ -1848,7 +1848,7 @@
         <v>5</v>
       </c>
       <c r="E26">
-        <v>55.9</v>
+        <v>57.7</v>
       </c>
       <c r="F26">
         <v>92.8</v>
@@ -1866,7 +1866,7 @@
         <v>36.6</v>
       </c>
       <c r="K26">
-        <v>44.2</v>
+        <v>28</v>
       </c>
       <c r="L26" t="s">
         <v>109</v>
@@ -1892,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="E27">
-        <v>8.4</v>
+        <v>7.6</v>
       </c>
       <c r="F27">
         <v>61.4</v>
@@ -1910,7 +1910,7 @@
         <v>19.7</v>
       </c>
       <c r="K27">
-        <v>58.8</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="L27" t="s">
         <v>111</v>
@@ -1936,7 +1936,7 @@
         <v>95</v>
       </c>
       <c r="E28">
-        <v>41.9</v>
+        <v>43.8</v>
       </c>
       <c r="F28">
         <v>29.2</v>
@@ -1954,7 +1954,7 @@
         <v>30.1</v>
       </c>
       <c r="K28">
-        <v>81.09999999999999</v>
+        <v>66.3</v>
       </c>
       <c r="L28" t="s">
         <v>110</v>
@@ -1980,7 +1980,7 @@
         <v>72.3</v>
       </c>
       <c r="E29">
-        <v>68.8</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="F29">
         <v>19.3</v>
@@ -1998,7 +1998,7 @@
         <v>89.7</v>
       </c>
       <c r="K29">
-        <v>93.8</v>
+        <v>85.59999999999999</v>
       </c>
       <c r="L29" t="s">
         <v>106</v>
@@ -2024,7 +2024,7 @@
         <v>48.5</v>
       </c>
       <c r="E30">
-        <v>75</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="F30">
         <v>31.9</v>
@@ -2042,7 +2042,7 @@
         <v>65.5</v>
       </c>
       <c r="K30">
-        <v>79.09999999999999</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="L30" t="s">
         <v>109</v>
@@ -2086,7 +2086,7 @@
         <v>74.59999999999999</v>
       </c>
       <c r="K31">
-        <v>76.8</v>
+        <v>60.8</v>
       </c>
       <c r="L31" t="s">
         <v>109</v>
@@ -2130,7 +2130,7 @@
         <v>92.3</v>
       </c>
       <c r="K32">
-        <v>37.5</v>
+        <v>58.2</v>
       </c>
       <c r="L32" t="s">
         <v>105</v>
@@ -2156,7 +2156,7 @@
         <v>78.59999999999999</v>
       </c>
       <c r="E33">
-        <v>42.1</v>
+        <v>40</v>
       </c>
       <c r="F33">
         <v>85.40000000000001</v>
@@ -2174,7 +2174,7 @@
         <v>30.7</v>
       </c>
       <c r="K33">
-        <v>6.4</v>
+        <v>5</v>
       </c>
       <c r="L33" t="s">
         <v>106</v>
@@ -2200,7 +2200,7 @@
         <v>10.4</v>
       </c>
       <c r="E34">
-        <v>40.4</v>
+        <v>37.9</v>
       </c>
       <c r="F34">
         <v>61.8</v>
@@ -2218,7 +2218,7 @@
         <v>46.3</v>
       </c>
       <c r="K34">
-        <v>27.2</v>
+        <v>15</v>
       </c>
       <c r="L34" t="s">
         <v>111</v>
@@ -2244,7 +2244,7 @@
         <v>88.5</v>
       </c>
       <c r="E35">
-        <v>92.59999999999999</v>
+        <v>93</v>
       </c>
       <c r="F35">
         <v>21.9</v>
@@ -2262,7 +2262,7 @@
         <v>94.2</v>
       </c>
       <c r="K35">
-        <v>95</v>
+        <v>91.7</v>
       </c>
       <c r="L35" t="s">
         <v>109</v>
@@ -2306,7 +2306,7 @@
         <v>20.2</v>
       </c>
       <c r="K36">
-        <v>27.2</v>
+        <v>15.1</v>
       </c>
       <c r="L36" t="s">
         <v>111</v>
@@ -2332,7 +2332,7 @@
         <v>45.8</v>
       </c>
       <c r="E37">
-        <v>56.4</v>
+        <v>54.1</v>
       </c>
       <c r="F37">
         <v>13.6</v>
@@ -2350,7 +2350,7 @@
         <v>71.2</v>
       </c>
       <c r="K37">
-        <v>67.7</v>
+        <v>50.3</v>
       </c>
       <c r="L37" t="s">
         <v>107</v>
@@ -2376,7 +2376,7 @@
         <v>5</v>
       </c>
       <c r="E38">
-        <v>46.5</v>
+        <v>44.2</v>
       </c>
       <c r="F38">
         <v>93.3</v>
@@ -2394,7 +2394,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="K38">
-        <v>71.40000000000001</v>
+        <v>54.4</v>
       </c>
       <c r="L38" t="s">
         <v>112</v>
@@ -2420,7 +2420,7 @@
         <v>11.2</v>
       </c>
       <c r="E39">
-        <v>65.8</v>
+        <v>63.2</v>
       </c>
       <c r="F39">
         <v>65</v>
@@ -2438,7 +2438,7 @@
         <v>81.90000000000001</v>
       </c>
       <c r="K39">
-        <v>63.7</v>
+        <v>46</v>
       </c>
       <c r="L39" t="s">
         <v>111</v>
@@ -2482,7 +2482,7 @@
         <v>52.6</v>
       </c>
       <c r="K40">
-        <v>65.90000000000001</v>
+        <v>48.4</v>
       </c>
       <c r="L40" t="s">
         <v>105</v>
@@ -2508,7 +2508,7 @@
         <v>85.90000000000001</v>
       </c>
       <c r="E41">
-        <v>36.5</v>
+        <v>35.8</v>
       </c>
       <c r="F41">
         <v>46.9</v>
@@ -2526,7 +2526,7 @@
         <v>64.90000000000001</v>
       </c>
       <c r="K41">
-        <v>74.09999999999999</v>
+        <v>57.5</v>
       </c>
       <c r="L41" t="s">
         <v>105</v>
@@ -2552,7 +2552,7 @@
         <v>44.8</v>
       </c>
       <c r="E42">
-        <v>71.40000000000001</v>
+        <v>69</v>
       </c>
       <c r="F42">
         <v>31.5</v>
@@ -2570,7 +2570,7 @@
         <v>88.8</v>
       </c>
       <c r="K42">
-        <v>67</v>
+        <v>79.7</v>
       </c>
       <c r="L42" t="s">
         <v>114</v>
@@ -2596,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="E43">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="F43">
         <v>59.7</v>
@@ -2614,7 +2614,7 @@
         <v>19.7</v>
       </c>
       <c r="K43">
-        <v>26.8</v>
+        <v>14.8</v>
       </c>
       <c r="L43" t="s">
         <v>115</v>
@@ -2640,7 +2640,7 @@
         <v>43.4</v>
       </c>
       <c r="E44">
-        <v>72.3</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="F44">
         <v>31.8</v>
@@ -2658,7 +2658,7 @@
         <v>89.40000000000001</v>
       </c>
       <c r="K44">
-        <v>78.5</v>
+        <v>88</v>
       </c>
       <c r="L44" t="s">
         <v>107</v>
@@ -2684,7 +2684,7 @@
         <v>92.2</v>
       </c>
       <c r="E45">
-        <v>51.3</v>
+        <v>53.9</v>
       </c>
       <c r="F45">
         <v>52.5</v>
@@ -2702,7 +2702,7 @@
         <v>86.2</v>
       </c>
       <c r="K45">
-        <v>79.3</v>
+        <v>88.2</v>
       </c>
       <c r="L45" t="s">
         <v>105</v>
@@ -2728,7 +2728,7 @@
         <v>57.3</v>
       </c>
       <c r="E46">
-        <v>65.90000000000001</v>
+        <v>68.2</v>
       </c>
       <c r="F46">
         <v>57</v>
@@ -2746,7 +2746,7 @@
         <v>70.5</v>
       </c>
       <c r="K46">
-        <v>44</v>
+        <v>27.8</v>
       </c>
       <c r="L46" t="s">
         <v>107</v>
@@ -2772,7 +2772,7 @@
         <v>52.2</v>
       </c>
       <c r="E47">
-        <v>14.5</v>
+        <v>16.3</v>
       </c>
       <c r="F47">
         <v>58.8</v>
@@ -2790,7 +2790,7 @@
         <v>5.9</v>
       </c>
       <c r="K47">
-        <v>10.9</v>
+        <v>20.9</v>
       </c>
       <c r="L47" t="s">
         <v>105</v>
@@ -2816,7 +2816,7 @@
         <v>58</v>
       </c>
       <c r="E48">
-        <v>53.6</v>
+        <v>50.9</v>
       </c>
       <c r="F48">
         <v>82.09999999999999</v>
@@ -2834,7 +2834,7 @@
         <v>19.2</v>
       </c>
       <c r="K48">
-        <v>6.1</v>
+        <v>5</v>
       </c>
       <c r="L48" t="s">
         <v>111</v>
@@ -2860,7 +2860,7 @@
         <v>67</v>
       </c>
       <c r="E49">
-        <v>43.5</v>
+        <v>41</v>
       </c>
       <c r="F49">
         <v>81.2</v>
@@ -2878,7 +2878,7 @@
         <v>5</v>
       </c>
       <c r="K49">
-        <v>6.2</v>
+        <v>14.4</v>
       </c>
       <c r="L49" t="s">
         <v>115</v>
@@ -2904,7 +2904,7 @@
         <v>75.40000000000001</v>
       </c>
       <c r="E50">
-        <v>36.1</v>
+        <v>38.5</v>
       </c>
       <c r="F50">
         <v>80.3</v>
@@ -2922,7 +2922,7 @@
         <v>68.3</v>
       </c>
       <c r="K50">
-        <v>42.5</v>
+        <v>59.3</v>
       </c>
       <c r="L50" t="s">
         <v>107</v>
@@ -2948,7 +2948,7 @@
         <v>30</v>
       </c>
       <c r="E51">
-        <v>7.3</v>
+        <v>6.6</v>
       </c>
       <c r="F51">
         <v>80.59999999999999</v>
@@ -2966,7 +2966,7 @@
         <v>17.5</v>
       </c>
       <c r="K51">
-        <v>24.7</v>
+        <v>39.5</v>
       </c>
       <c r="L51" t="s">
         <v>111</v>
@@ -2992,7 +2992,7 @@
         <v>81.5</v>
       </c>
       <c r="E52">
-        <v>39</v>
+        <v>37.5</v>
       </c>
       <c r="F52">
         <v>94.40000000000001</v>
@@ -3010,7 +3010,7 @@
         <v>6.7</v>
       </c>
       <c r="K52">
-        <v>6.9</v>
+        <v>14.9</v>
       </c>
       <c r="L52" t="s">
         <v>105</v>
@@ -3036,7 +3036,7 @@
         <v>13.6</v>
       </c>
       <c r="E53">
-        <v>63.8</v>
+        <v>61.3</v>
       </c>
       <c r="F53">
         <v>38.8</v>
@@ -3054,7 +3054,7 @@
         <v>80.59999999999999</v>
       </c>
       <c r="K53">
-        <v>61.5</v>
+        <v>76.2</v>
       </c>
       <c r="L53" t="s">
         <v>115</v>
@@ -3080,7 +3080,7 @@
         <v>35.4</v>
       </c>
       <c r="E54">
-        <v>48.2</v>
+        <v>45.6</v>
       </c>
       <c r="F54">
         <v>82.90000000000001</v>
@@ -3098,7 +3098,7 @@
         <v>21.6</v>
       </c>
       <c r="K54">
-        <v>6.2</v>
+        <v>5</v>
       </c>
       <c r="L54" t="s">
         <v>112</v>
@@ -3124,7 +3124,7 @@
         <v>71.90000000000001</v>
       </c>
       <c r="E55">
-        <v>64</v>
+        <v>63.7</v>
       </c>
       <c r="F55">
         <v>88.8</v>
@@ -3142,7 +3142,7 @@
         <v>65.90000000000001</v>
       </c>
       <c r="K55">
-        <v>65</v>
+        <v>47.4</v>
       </c>
       <c r="L55" t="s">
         <v>107</v>
@@ -3168,7 +3168,7 @@
         <v>32.4</v>
       </c>
       <c r="E56">
-        <v>74.2</v>
+        <v>71.90000000000001</v>
       </c>
       <c r="F56">
         <v>93</v>
@@ -3186,7 +3186,7 @@
         <v>23.2</v>
       </c>
       <c r="K56">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="L56" t="s">
         <v>115</v>
@@ -3230,7 +3230,7 @@
         <v>91.3</v>
       </c>
       <c r="K57">
-        <v>31.6</v>
+        <v>48.7</v>
       </c>
       <c r="L57" t="s">
         <v>107</v>
@@ -3274,7 +3274,7 @@
         <v>69</v>
       </c>
       <c r="K58">
-        <v>82.09999999999999</v>
+        <v>90.3</v>
       </c>
       <c r="L58" t="s">
         <v>109</v>
@@ -3318,7 +3318,7 @@
         <v>87.40000000000001</v>
       </c>
       <c r="K59">
-        <v>66.3</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="L59" t="s">
         <v>115</v>
@@ -3344,7 +3344,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="E60">
-        <v>48.2</v>
+        <v>50.1</v>
       </c>
       <c r="F60">
         <v>58.2</v>
@@ -3362,7 +3362,7 @@
         <v>86.40000000000001</v>
       </c>
       <c r="K60">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="L60" t="s">
         <v>105</v>
@@ -3388,7 +3388,7 @@
         <v>46.9</v>
       </c>
       <c r="E61">
-        <v>44.1</v>
+        <v>42.5</v>
       </c>
       <c r="F61">
         <v>60.6</v>
@@ -3406,7 +3406,7 @@
         <v>27.7</v>
       </c>
       <c r="K61">
-        <v>6.9</v>
+        <v>15.5</v>
       </c>
       <c r="L61" t="s">
         <v>105</v>
@@ -3432,7 +3432,7 @@
         <v>33.2</v>
       </c>
       <c r="E62">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="F62">
         <v>38</v>
@@ -3450,7 +3450,7 @@
         <v>45.1</v>
       </c>
       <c r="K62">
-        <v>59.1</v>
+        <v>41.5</v>
       </c>
       <c r="L62" t="s">
         <v>115</v>
@@ -3494,7 +3494,7 @@
         <v>21.1</v>
       </c>
       <c r="K63">
-        <v>6.2</v>
+        <v>5</v>
       </c>
       <c r="L63" t="s">
         <v>106</v>
@@ -3520,7 +3520,7 @@
         <v>43.5</v>
       </c>
       <c r="E64">
-        <v>38.6</v>
+        <v>39.8</v>
       </c>
       <c r="F64">
         <v>95</v>
@@ -3538,7 +3538,7 @@
         <v>8.699999999999999</v>
       </c>
       <c r="K64">
-        <v>9.300000000000001</v>
+        <v>20.9</v>
       </c>
       <c r="L64" t="s">
         <v>107</v>
@@ -3564,7 +3564,7 @@
         <v>35.8</v>
       </c>
       <c r="E65">
-        <v>32.6</v>
+        <v>30.5</v>
       </c>
       <c r="F65">
         <v>63.3</v>
@@ -3582,7 +3582,7 @@
         <v>23.2</v>
       </c>
       <c r="K65">
-        <v>6.2</v>
+        <v>13.8</v>
       </c>
       <c r="L65" t="s">
         <v>114</v>
@@ -3608,7 +3608,7 @@
         <v>79.7</v>
       </c>
       <c r="E66">
-        <v>34.9</v>
+        <v>38.3</v>
       </c>
       <c r="F66">
         <v>20.2</v>
@@ -3626,7 +3626,7 @@
         <v>59.6</v>
       </c>
       <c r="K66">
-        <v>75.3</v>
+        <v>59</v>
       </c>
       <c r="L66" t="s">
         <v>109</v>
@@ -3652,7 +3652,7 @@
         <v>82.2</v>
       </c>
       <c r="E67">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="F67">
         <v>36.4</v>
@@ -3670,7 +3670,7 @@
         <v>5.4</v>
       </c>
       <c r="K67">
-        <v>26</v>
+        <v>14.2</v>
       </c>
       <c r="L67" t="s">
         <v>105</v>
@@ -3696,7 +3696,7 @@
         <v>81.09999999999999</v>
       </c>
       <c r="E68">
-        <v>21.4</v>
+        <v>23.6</v>
       </c>
       <c r="F68">
         <v>42.1</v>
@@ -3714,7 +3714,7 @@
         <v>25.8</v>
       </c>
       <c r="K68">
-        <v>77.7</v>
+        <v>61.9</v>
       </c>
       <c r="L68" t="s">
         <v>109</v>
@@ -3740,7 +3740,7 @@
         <v>85.2</v>
       </c>
       <c r="E69">
-        <v>28.5</v>
+        <v>29.9</v>
       </c>
       <c r="F69">
         <v>61.2</v>
@@ -3758,7 +3758,7 @@
         <v>19.4</v>
       </c>
       <c r="K69">
-        <v>32.3</v>
+        <v>18.7</v>
       </c>
       <c r="L69" t="s">
         <v>105</v>
@@ -3784,7 +3784,7 @@
         <v>84.59999999999999</v>
       </c>
       <c r="E70">
-        <v>72.2</v>
+        <v>73.7</v>
       </c>
       <c r="F70">
         <v>86.2</v>
@@ -3802,7 +3802,7 @@
         <v>73.09999999999999</v>
       </c>
       <c r="K70">
-        <v>45.2</v>
+        <v>28.8</v>
       </c>
       <c r="L70" t="s">
         <v>107</v>
@@ -3828,7 +3828,7 @@
         <v>22.9</v>
       </c>
       <c r="E71">
-        <v>28.4</v>
+        <v>45.7</v>
       </c>
       <c r="F71">
         <v>28.8</v>
@@ -3846,7 +3846,7 @@
         <v>74.8</v>
       </c>
       <c r="K71">
-        <v>95</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="L71" t="s">
         <v>109</v>
@@ -3872,7 +3872,7 @@
         <v>5</v>
       </c>
       <c r="E72">
-        <v>53.6</v>
+        <v>51</v>
       </c>
       <c r="F72">
         <v>5</v>
@@ -3890,7 +3890,7 @@
         <v>85.3</v>
       </c>
       <c r="K72">
-        <v>91.8</v>
+        <v>82</v>
       </c>
       <c r="L72" t="s">
         <v>111</v>
@@ -3934,7 +3934,7 @@
         <v>20</v>
       </c>
       <c r="K73">
-        <v>6.2</v>
+        <v>15.2</v>
       </c>
       <c r="L73" t="s">
         <v>108</v>
@@ -3960,7 +3960,7 @@
         <v>48.3</v>
       </c>
       <c r="E74">
-        <v>18.2</v>
+        <v>18.3</v>
       </c>
       <c r="F74">
         <v>94.59999999999999</v>
@@ -3978,7 +3978,7 @@
         <v>25.3</v>
       </c>
       <c r="K74">
-        <v>8.1</v>
+        <v>17.9</v>
       </c>
       <c r="L74" t="s">
         <v>105</v>
@@ -4004,7 +4004,7 @@
         <v>11.4</v>
       </c>
       <c r="E75">
-        <v>34.7</v>
+        <v>33.1</v>
       </c>
       <c r="F75">
         <v>94.09999999999999</v>
@@ -4022,7 +4022,7 @@
         <v>62.9</v>
       </c>
       <c r="K75">
-        <v>61.9</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="L75" t="s">
         <v>107</v>
@@ -4092,7 +4092,7 @@
         <v>89.5</v>
       </c>
       <c r="E77">
-        <v>83.2</v>
+        <v>82.5</v>
       </c>
       <c r="F77">
         <v>82.90000000000001</v>
@@ -4110,7 +4110,7 @@
         <v>60.1</v>
       </c>
       <c r="K77">
-        <v>7.7</v>
+        <v>17.2</v>
       </c>
       <c r="L77" t="s">
         <v>105</v>
@@ -4136,7 +4136,7 @@
         <v>32.6</v>
       </c>
       <c r="E78">
-        <v>33</v>
+        <v>30.8</v>
       </c>
       <c r="F78">
         <v>5.1</v>
@@ -4154,7 +4154,7 @@
         <v>25</v>
       </c>
       <c r="K78">
-        <v>63.1</v>
+        <v>78.3</v>
       </c>
       <c r="L78" t="s">
         <v>114</v>
@@ -4180,7 +4180,7 @@
         <v>13.6</v>
       </c>
       <c r="E79">
-        <v>18.8</v>
+        <v>17.3</v>
       </c>
       <c r="F79">
         <v>60.5</v>
@@ -4198,7 +4198,7 @@
         <v>23.8</v>
       </c>
       <c r="K79">
-        <v>6.2</v>
+        <v>13.6</v>
       </c>
       <c r="L79" t="s">
         <v>115</v>
@@ -4224,7 +4224,7 @@
         <v>13</v>
       </c>
       <c r="E80">
-        <v>67.2</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="F80">
         <v>60.4</v>
@@ -4242,7 +4242,7 @@
         <v>82.3</v>
       </c>
       <c r="K80">
-        <v>30</v>
+        <v>46.3</v>
       </c>
       <c r="L80" t="s">
         <v>115</v>
@@ -4268,7 +4268,7 @@
         <v>21.7</v>
       </c>
       <c r="E81">
-        <v>58.5</v>
+        <v>61.9</v>
       </c>
       <c r="F81">
         <v>10.5</v>
@@ -4286,7 +4286,7 @@
         <v>69.8</v>
       </c>
       <c r="K81">
-        <v>85.09999999999999</v>
+        <v>71.8</v>
       </c>
       <c r="L81" t="s">
         <v>109</v>
@@ -4312,7 +4312,7 @@
         <v>5</v>
       </c>
       <c r="E82">
-        <v>55.3</v>
+        <v>58.1</v>
       </c>
       <c r="F82">
         <v>95</v>
@@ -4330,7 +4330,7 @@
         <v>53.6</v>
       </c>
       <c r="K82">
-        <v>39.2</v>
+        <v>55.7</v>
       </c>
       <c r="L82" t="s">
         <v>109</v>
@@ -4356,7 +4356,7 @@
         <v>95</v>
       </c>
       <c r="E83">
-        <v>91.7</v>
+        <v>92.2</v>
       </c>
       <c r="F83">
         <v>5.7</v>
@@ -4400,7 +4400,7 @@
         <v>32.5</v>
       </c>
       <c r="E84">
-        <v>40.9</v>
+        <v>38.4</v>
       </c>
       <c r="F84">
         <v>82.59999999999999</v>
@@ -4418,7 +4418,7 @@
         <v>18.5</v>
       </c>
       <c r="K84">
-        <v>57.4</v>
+        <v>72.5</v>
       </c>
       <c r="L84" t="s">
         <v>111</v>
@@ -4444,7 +4444,7 @@
         <v>95</v>
       </c>
       <c r="E85">
-        <v>83.7</v>
+        <v>83</v>
       </c>
       <c r="F85">
         <v>10.7</v>
@@ -4462,7 +4462,7 @@
         <v>88.59999999999999</v>
       </c>
       <c r="K85">
-        <v>76.5</v>
+        <v>60.4</v>
       </c>
       <c r="L85" t="s">
         <v>105</v>
@@ -4488,7 +4488,7 @@
         <v>32.3</v>
       </c>
       <c r="E86">
-        <v>26.4</v>
+        <v>24.4</v>
       </c>
       <c r="F86">
         <v>16.3</v>
@@ -4506,7 +4506,7 @@
         <v>19.8</v>
       </c>
       <c r="K86">
-        <v>26.2</v>
+        <v>41.4</v>
       </c>
       <c r="L86" t="s">
         <v>111</v>
@@ -4532,7 +4532,7 @@
         <v>76.59999999999999</v>
       </c>
       <c r="E87">
-        <v>31.5</v>
+        <v>30</v>
       </c>
       <c r="F87">
         <v>35.4</v>
@@ -4550,7 +4550,7 @@
         <v>20</v>
       </c>
       <c r="K87">
-        <v>60</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="L87" t="s">
         <v>105</v>
@@ -4576,7 +4576,7 @@
         <v>78.3</v>
       </c>
       <c r="E88">
-        <v>69.40000000000001</v>
+        <v>71</v>
       </c>
       <c r="F88">
         <v>7.2</v>
@@ -4594,7 +4594,7 @@
         <v>66.7</v>
       </c>
       <c r="K88">
-        <v>83.7</v>
+        <v>69.7</v>
       </c>
       <c r="L88" t="s">
         <v>109</v>
@@ -4620,7 +4620,7 @@
         <v>76.40000000000001</v>
       </c>
       <c r="E89">
-        <v>72.40000000000001</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="F89">
         <v>58.7</v>
@@ -4638,7 +4638,7 @@
         <v>35.1</v>
       </c>
       <c r="K89">
-        <v>39.9</v>
+        <v>58.1</v>
       </c>
       <c r="L89" t="s">
         <v>107</v>
@@ -4664,7 +4664,7 @@
         <v>31.5</v>
       </c>
       <c r="E90">
-        <v>27.9</v>
+        <v>25.9</v>
       </c>
       <c r="F90">
         <v>35.2</v>
@@ -4682,7 +4682,7 @@
         <v>18.3</v>
       </c>
       <c r="K90">
-        <v>25.8</v>
+        <v>40.5</v>
       </c>
       <c r="L90" t="s">
         <v>115</v>
@@ -4708,7 +4708,7 @@
         <v>85.2</v>
       </c>
       <c r="E91">
-        <v>42.8</v>
+        <v>43.5</v>
       </c>
       <c r="F91">
         <v>35.2</v>
@@ -4726,7 +4726,7 @@
         <v>17.9</v>
       </c>
       <c r="K91">
-        <v>8.800000000000001</v>
+        <v>5</v>
       </c>
       <c r="L91" t="s">
         <v>105</v>
@@ -4752,7 +4752,7 @@
         <v>84.7</v>
       </c>
       <c r="E92">
-        <v>50.9</v>
+        <v>49.1</v>
       </c>
       <c r="F92">
         <v>59.3</v>
@@ -4770,7 +4770,7 @@
         <v>22.5</v>
       </c>
       <c r="K92">
-        <v>26.9</v>
+        <v>41.9</v>
       </c>
       <c r="L92" t="s">
         <v>105</v>

</xml_diff>